<commit_message>
opdracht 2 opgesplits vanwege geprojecteerde fatala fout-afloop
</commit_message>
<xml_diff>
--- a/1.0.4-rc/Validatiematrix 1 (version 1).xlsb.xlsx
+++ b/1.0.4-rc/Validatiematrix 1 (version 1).xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_validatietestcontent\1.0.4-rc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F00B1E8-196F-4FCD-8D58-B29CE5546B0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15C0116-5B58-452C-A02E-934E9AC5953F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7800" uniqueCount="1258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7801" uniqueCount="1257">
   <si>
     <t>Is Opdracht.zip een geldige zip</t>
   </si>
@@ -3831,9 +3831,6 @@
   </si>
   <si>
     <t>(Geonovum) DatumBekendmaking-fout (LVBB1511)</t>
-  </si>
-  <si>
-    <t>(Geonovum) Nog te testen zodra we een Digikoppeling zonder transformaties hebben.</t>
   </si>
   <si>
     <t>(Geonovum) kijken hoe en wat.</t>
@@ -5406,9 +5403,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S585"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N58" sqref="N58"/>
+      <selection pane="bottomLeft" activeCell="P42" sqref="P42:S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5480,7 +5477,7 @@
         <v>1234</v>
       </c>
       <c r="R1" s="45" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="S1" s="43" t="s">
         <v>1233</v>
@@ -6383,7 +6380,7 @@
         <v>44166</v>
       </c>
       <c r="R20" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S20" s="21" t="s">
         <v>1237</v>
@@ -6440,7 +6437,7 @@
         <v>44166</v>
       </c>
       <c r="R21" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S21" s="21" t="s">
         <v>1237</v>
@@ -6497,7 +6494,7 @@
         <v>44166</v>
       </c>
       <c r="R22" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S22" s="21" t="s">
         <v>1237</v>
@@ -6554,7 +6551,7 @@
         <v>44166</v>
       </c>
       <c r="R23" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S23" s="21" t="s">
         <v>1237</v>
@@ -6611,7 +6608,7 @@
         <v>44166</v>
       </c>
       <c r="R24" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S24" s="21" t="s">
         <v>1237</v>
@@ -6668,7 +6665,7 @@
         <v>44166</v>
       </c>
       <c r="R25" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S25" s="21" t="s">
         <v>1237</v>
@@ -6725,7 +6722,7 @@
         <v>44166</v>
       </c>
       <c r="R26" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S26" s="21" t="s">
         <v>1237</v>
@@ -6782,7 +6779,7 @@
         <v>44166</v>
       </c>
       <c r="R27" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S27" s="21" t="s">
         <v>1237</v>
@@ -6839,7 +6836,7 @@
         <v>44166</v>
       </c>
       <c r="R28" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S28" s="21" t="s">
         <v>1237</v>
@@ -6896,7 +6893,7 @@
         <v>44166</v>
       </c>
       <c r="R29" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S29" s="21" t="s">
         <v>1237</v>
@@ -6953,7 +6950,7 @@
         <v>44166</v>
       </c>
       <c r="R30" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S30" s="21" t="s">
         <v>1237</v>
@@ -7010,7 +7007,7 @@
         <v>44166</v>
       </c>
       <c r="R31" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S31" s="21" t="s">
         <v>1237</v>
@@ -7067,7 +7064,7 @@
         <v>44166</v>
       </c>
       <c r="R32" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S32" s="21" t="s">
         <v>1237</v>
@@ -7124,7 +7121,7 @@
         <v>44166</v>
       </c>
       <c r="R33" s="46" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S33" s="21" t="s">
         <v>1237</v>
@@ -7384,7 +7381,7 @@
       </c>
       <c r="R38" s="46"/>
       <c r="S38" s="21" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7441,7 +7438,7 @@
       </c>
       <c r="R39" s="46"/>
       <c r="S39" s="21" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7498,10 +7495,10 @@
       </c>
       <c r="R40" s="46"/>
       <c r="S40" s="21" t="s">
-        <v>1256</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="27">
         <v>1</v>
       </c>
@@ -7542,17 +7539,23 @@
         <v>25</v>
       </c>
       <c r="N41" s="11" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="O41" s="11" t="s">
         <v>1066</v>
       </c>
-      <c r="P41" s="21"/>
-      <c r="Q41" s="46"/>
+      <c r="P41" s="21">
+        <v>500</v>
+      </c>
+      <c r="Q41" s="46">
+        <v>44167</v>
+      </c>
       <c r="R41" s="46"/>
-      <c r="S41" s="21"/>
-    </row>
-    <row r="42" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S41" s="21" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27">
         <v>1</v>
       </c>
@@ -7598,15 +7601,15 @@
       <c r="O42" s="11" t="s">
         <v>1066</v>
       </c>
-      <c r="P42" s="21" t="s">
-        <v>1236</v>
+      <c r="P42" s="21">
+        <v>500</v>
       </c>
       <c r="Q42" s="46">
-        <v>44166</v>
+        <v>44167</v>
       </c>
       <c r="R42" s="46"/>
       <c r="S42" s="21" t="s">
-        <v>1248</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7660,7 +7663,7 @@
       <c r="R43" s="46"/>
       <c r="S43" s="21"/>
     </row>
-    <row r="44" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27">
         <v>1</v>
       </c>
@@ -7706,15 +7709,15 @@
       <c r="O44" s="11" t="s">
         <v>1066</v>
       </c>
-      <c r="P44" s="21" t="s">
-        <v>1236</v>
+      <c r="P44" s="21">
+        <v>500</v>
       </c>
       <c r="Q44" s="46">
-        <v>44166</v>
+        <v>44167</v>
       </c>
       <c r="R44" s="46"/>
       <c r="S44" s="21" t="s">
-        <v>1248</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7821,7 +7824,7 @@
         <v>44166</v>
       </c>
       <c r="R46" s="46" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="S46" s="21" t="s">
         <v>1238</v>
@@ -7880,7 +7883,7 @@
         <v>44166</v>
       </c>
       <c r="R47" s="46" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="S47" s="21" t="s">
         <v>1239</v>
@@ -7990,10 +7993,10 @@
         <v>44166</v>
       </c>
       <c r="R49" s="46" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="S49" s="21" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8049,7 +8052,7 @@
         <v>44166</v>
       </c>
       <c r="R50" s="46" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="S50" s="21" t="s">
         <v>1235</v>
@@ -8494,10 +8497,16 @@
       <c r="O58" s="21" t="s">
         <v>1067</v>
       </c>
-      <c r="P58" s="21"/>
-      <c r="Q58" s="46"/>
+      <c r="P58" s="21">
+        <v>500</v>
+      </c>
+      <c r="Q58" s="46">
+        <v>44167</v>
+      </c>
       <c r="R58" s="46"/>
-      <c r="S58" s="21"/>
+      <c r="S58" s="21" t="s">
+        <v>1255</v>
+      </c>
     </row>
     <row r="59" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="26">
@@ -8545,10 +8554,16 @@
       <c r="O59" s="21" t="s">
         <v>1067</v>
       </c>
-      <c r="P59" s="21"/>
-      <c r="Q59" s="46"/>
+      <c r="P59" s="21">
+        <v>500</v>
+      </c>
+      <c r="Q59" s="46">
+        <v>44167</v>
+      </c>
       <c r="R59" s="46"/>
-      <c r="S59" s="21"/>
+      <c r="S59" s="21" t="s">
+        <v>1255</v>
+      </c>
     </row>
     <row r="60" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="26">
@@ -20977,7 +20992,7 @@
       </c>
       <c r="R302" s="46"/>
       <c r="S302" s="21" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="303" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22209,7 +22224,7 @@
       </c>
       <c r="R326" s="46"/>
       <c r="S326" s="21" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="327" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22374,7 +22389,7 @@
       </c>
       <c r="R329" s="46"/>
       <c r="S329" s="21" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="330" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22539,7 +22554,7 @@
       </c>
       <c r="R332" s="46"/>
       <c r="S332" s="21" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="333" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -34655,6 +34670,7 @@
     <filterColumn colId="13">
       <filters>
         <filter val="opdracht_3"/>
+        <filter val="opdracht_4"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
bezig met wordt-akn opdracht_11
</commit_message>
<xml_diff>
--- a/1.0.4-rc/Validatiematrix 1 (version 1).xlsb.xlsx
+++ b/1.0.4-rc/Validatiematrix 1 (version 1).xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_validatietestcontent\1.0.4-rc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A912BA-140E-408C-AF27-3D29E8B377BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F580DB-291E-4917-AC41-88B0A4E83F08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="330" windowWidth="29040" windowHeight="15990" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7836" uniqueCount="1263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7834" uniqueCount="1262">
   <si>
     <t>Is Opdracht.zip een geldige zip</t>
   </si>
@@ -3738,9 +3738,6 @@
     <t>geo-validatie</t>
   </si>
   <si>
-    <t>opdracht_9</t>
-  </si>
-  <si>
     <t>opdracht_10</t>
   </si>
   <si>
@@ -3750,9 +3747,6 @@
     <t>opdracht_11</t>
   </si>
   <si>
-    <t>opdracht_10 en 11</t>
-  </si>
-  <si>
     <t>opdracht_12</t>
   </si>
   <si>
@@ -3844,6 +3838,9 @@
   </si>
   <si>
     <t>Internal Server Error</t>
+  </si>
+  <si>
+    <t>opdracht_17</t>
   </si>
   <si>
     <t>opdracht_lvbb1002</t>
@@ -5422,9 +5419,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S585"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P65" sqref="P65:P162"/>
+      <selection pane="bottomLeft" activeCell="N167" sqref="N167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5490,16 +5487,16 @@
         <v>1065</v>
       </c>
       <c r="P1" s="43" t="s">
+        <v>1229</v>
+      </c>
+      <c r="Q1" s="45" t="s">
+        <v>1232</v>
+      </c>
+      <c r="R1" s="45" t="s">
+        <v>1244</v>
+      </c>
+      <c r="S1" s="43" t="s">
         <v>1231</v>
-      </c>
-      <c r="Q1" s="45" t="s">
-        <v>1234</v>
-      </c>
-      <c r="R1" s="45" t="s">
-        <v>1246</v>
-      </c>
-      <c r="S1" s="43" t="s">
-        <v>1233</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6393,16 +6390,16 @@
       </c>
       <c r="O20" s="21"/>
       <c r="P20" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q20" s="46">
         <v>44166</v>
       </c>
       <c r="R20" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S20" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6450,16 +6447,16 @@
       </c>
       <c r="O21" s="21"/>
       <c r="P21" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q21" s="46">
         <v>44166</v>
       </c>
       <c r="R21" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S21" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6507,16 +6504,16 @@
       </c>
       <c r="O22" s="21"/>
       <c r="P22" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q22" s="46">
         <v>44166</v>
       </c>
       <c r="R22" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S22" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6564,16 +6561,16 @@
       </c>
       <c r="O23" s="11"/>
       <c r="P23" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q23" s="46">
         <v>44166</v>
       </c>
       <c r="R23" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S23" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6621,16 +6618,16 @@
       </c>
       <c r="O24" s="11"/>
       <c r="P24" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q24" s="46">
         <v>44166</v>
       </c>
       <c r="R24" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S24" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6678,16 +6675,16 @@
       </c>
       <c r="O25" s="11"/>
       <c r="P25" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q25" s="46">
         <v>44166</v>
       </c>
       <c r="R25" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S25" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6735,16 +6732,16 @@
       </c>
       <c r="O26" s="11"/>
       <c r="P26" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q26" s="46">
         <v>44166</v>
       </c>
       <c r="R26" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S26" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6792,16 +6789,16 @@
       </c>
       <c r="O27" s="11"/>
       <c r="P27" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q27" s="46">
         <v>44166</v>
       </c>
       <c r="R27" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S27" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6849,16 +6846,16 @@
       </c>
       <c r="O28" s="11"/>
       <c r="P28" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q28" s="46">
         <v>44166</v>
       </c>
       <c r="R28" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S28" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6906,16 +6903,16 @@
       </c>
       <c r="O29" s="11"/>
       <c r="P29" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q29" s="46">
         <v>44166</v>
       </c>
       <c r="R29" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S29" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6963,16 +6960,16 @@
       </c>
       <c r="O30" s="11"/>
       <c r="P30" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q30" s="46">
         <v>44166</v>
       </c>
       <c r="R30" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S30" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7020,16 +7017,16 @@
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q31" s="46">
         <v>44166</v>
       </c>
       <c r="R31" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S31" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7077,16 +7074,16 @@
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q32" s="46">
         <v>44166</v>
       </c>
       <c r="R32" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S32" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7134,16 +7131,16 @@
       </c>
       <c r="O33" s="11"/>
       <c r="P33" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q33" s="46">
         <v>44166</v>
       </c>
       <c r="R33" s="46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S33" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7387,7 +7384,7 @@
         <v>25</v>
       </c>
       <c r="N38" s="11" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="O38" s="11" t="s">
         <v>1066</v>
@@ -7400,7 +7397,7 @@
       </c>
       <c r="R38" s="46"/>
       <c r="S38" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7444,7 +7441,7 @@
         <v>25</v>
       </c>
       <c r="N39" s="11" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="O39" s="11" t="s">
         <v>1066</v>
@@ -7457,7 +7454,7 @@
       </c>
       <c r="R39" s="46"/>
       <c r="S39" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7501,7 +7498,7 @@
         <v>25</v>
       </c>
       <c r="N40" s="11" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="O40" s="11" t="s">
         <v>1066</v>
@@ -7514,7 +7511,7 @@
       </c>
       <c r="R40" s="46"/>
       <c r="S40" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7558,7 +7555,7 @@
         <v>25</v>
       </c>
       <c r="N41" s="11" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="O41" s="11" t="s">
         <v>1066</v>
@@ -7571,7 +7568,7 @@
       </c>
       <c r="R41" s="46"/>
       <c r="S41" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7615,7 +7612,7 @@
         <v>25</v>
       </c>
       <c r="N42" s="11" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="O42" s="11" t="s">
         <v>1066</v>
@@ -7628,7 +7625,7 @@
       </c>
       <c r="R42" s="46"/>
       <c r="S42" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7672,7 +7669,7 @@
         <v>25</v>
       </c>
       <c r="N43" s="11" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="O43" s="11" t="s">
         <v>1066</v>
@@ -7685,7 +7682,7 @@
       </c>
       <c r="R43" s="46"/>
       <c r="S43" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7729,7 +7726,7 @@
         <v>25</v>
       </c>
       <c r="N44" s="11" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="O44" s="11" t="s">
         <v>1066</v>
@@ -7742,7 +7739,7 @@
       </c>
       <c r="R44" s="46"/>
       <c r="S44" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7786,7 +7783,7 @@
         <v>25</v>
       </c>
       <c r="N45" s="11" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="O45" s="11" t="s">
         <v>1066</v>
@@ -7799,7 +7796,7 @@
       </c>
       <c r="R45" s="46"/>
       <c r="S45" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="46" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7849,16 +7846,16 @@
         <v>1067</v>
       </c>
       <c r="P46" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q46" s="46">
         <v>44166</v>
       </c>
       <c r="R46" s="46" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="S46" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7908,16 +7905,16 @@
         <v>1067</v>
       </c>
       <c r="P47" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q47" s="46">
         <v>44166</v>
       </c>
       <c r="R47" s="46" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="S47" s="21" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7961,7 +7958,7 @@
         <v>25</v>
       </c>
       <c r="N48" s="11" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="O48" s="11" t="s">
         <v>1066</v>
@@ -7974,7 +7971,7 @@
       </c>
       <c r="R48" s="46"/>
       <c r="S48" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="49" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8024,16 +8021,16 @@
         <v>1067</v>
       </c>
       <c r="P49" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q49" s="46">
         <v>44166</v>
       </c>
       <c r="R49" s="46" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="S49" s="21" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8083,16 +8080,16 @@
         <v>1067</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="Q50" s="46">
         <v>44166</v>
       </c>
       <c r="R50" s="46" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="S50" s="21" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8136,7 +8133,7 @@
         <v>25</v>
       </c>
       <c r="N51" s="11" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="O51" s="11" t="s">
         <v>1066</v>
@@ -8149,7 +8146,7 @@
       </c>
       <c r="R51" s="46"/>
       <c r="S51" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8199,14 +8196,14 @@
         <v>1067</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q52" s="46">
         <v>44166</v>
       </c>
       <c r="R52" s="46"/>
       <c r="S52" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8256,14 +8253,14 @@
         <v>1067</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q53" s="46">
         <v>44166</v>
       </c>
       <c r="R53" s="46"/>
       <c r="S53" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="54" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8313,14 +8310,14 @@
         <v>1067</v>
       </c>
       <c r="P54" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q54" s="46">
         <v>44166</v>
       </c>
       <c r="R54" s="46"/>
       <c r="S54" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="55" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8370,14 +8367,14 @@
         <v>1067</v>
       </c>
       <c r="P55" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q55" s="46">
         <v>44166</v>
       </c>
       <c r="R55" s="46"/>
       <c r="S55" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="56" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8427,14 +8424,14 @@
         <v>1067</v>
       </c>
       <c r="P56" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q56" s="46">
         <v>44166</v>
       </c>
       <c r="R56" s="46"/>
       <c r="S56" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="57" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8484,14 +8481,14 @@
         <v>1067</v>
       </c>
       <c r="P57" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q57" s="46">
         <v>44166</v>
       </c>
       <c r="R57" s="46"/>
       <c r="S57" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="58" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8535,7 +8532,7 @@
         <v>25</v>
       </c>
       <c r="N58" s="21" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="O58" s="21" t="s">
         <v>1067</v>
@@ -8548,7 +8545,7 @@
       </c>
       <c r="R58" s="46"/>
       <c r="S58" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="59" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8592,7 +8589,7 @@
         <v>25</v>
       </c>
       <c r="N59" s="21" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="O59" s="21" t="s">
         <v>1067</v>
@@ -8605,7 +8602,7 @@
       </c>
       <c r="R59" s="46"/>
       <c r="S59" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="60" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8749,7 +8746,7 @@
       <c r="R62" s="46"/>
       <c r="S62" s="21"/>
     </row>
-    <row r="63" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="28">
         <v>2</v>
       </c>
@@ -8803,7 +8800,7 @@
       </c>
       <c r="R63" s="46"/>
       <c r="S63" s="21" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="64" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8853,7 +8850,7 @@
       <c r="R64" s="46"/>
       <c r="S64" s="21"/>
     </row>
-    <row r="65" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="29">
         <v>2</v>
       </c>
@@ -8907,7 +8904,7 @@
       </c>
       <c r="R65" s="46"/>
       <c r="S65" s="21" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="66" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9016,7 +9013,7 @@
       <c r="A68" s="29">
         <v>2</v>
       </c>
-      <c r="B68" s="26" t="s">
+      <c r="B68" s="15" t="s">
         <v>156</v>
       </c>
       <c r="C68" s="21" t="s">
@@ -9353,7 +9350,7 @@
       <c r="R74" s="46"/>
       <c r="S74" s="21"/>
     </row>
-    <row r="75" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="29">
         <v>2</v>
       </c>
@@ -9407,7 +9404,7 @@
       </c>
       <c r="R75" s="46"/>
       <c r="S75" s="21" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="76" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9826,9 +9823,7 @@
       <c r="M84" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="N84" s="11" t="s">
-        <v>1216</v>
-      </c>
+      <c r="N84" s="11"/>
       <c r="O84" s="11" t="s">
         <v>1067</v>
       </c>
@@ -9931,14 +9926,14 @@
         <v>1067</v>
       </c>
       <c r="P86" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q86" s="46">
         <v>44166</v>
       </c>
       <c r="R86" s="46"/>
       <c r="S86" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="87" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9988,7 +9983,7 @@
       <c r="R87" s="46"/>
       <c r="S87" s="21"/>
     </row>
-    <row r="88" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="26">
         <v>2</v>
       </c>
@@ -10042,10 +10037,10 @@
       </c>
       <c r="R88" s="46"/>
       <c r="S88" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="89" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="26">
         <v>2</v>
       </c>
@@ -10099,10 +10094,10 @@
       </c>
       <c r="R89" s="46"/>
       <c r="S89" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="90" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="26">
         <v>2</v>
       </c>
@@ -10156,10 +10151,10 @@
       </c>
       <c r="R90" s="46"/>
       <c r="S90" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="91" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="26">
         <v>2</v>
       </c>
@@ -10213,10 +10208,10 @@
       </c>
       <c r="R91" s="46"/>
       <c r="S91" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="92" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="26">
         <v>2</v>
       </c>
@@ -10270,10 +10265,10 @@
       </c>
       <c r="R92" s="46"/>
       <c r="S92" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="93" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="26">
         <v>2</v>
       </c>
@@ -10327,10 +10322,10 @@
       </c>
       <c r="R93" s="46"/>
       <c r="S93" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="94" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="26">
         <v>2</v>
       </c>
@@ -10384,10 +10379,10 @@
       </c>
       <c r="R94" s="46"/>
       <c r="S94" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="95" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="26">
         <v>2</v>
       </c>
@@ -10441,10 +10436,10 @@
       </c>
       <c r="R95" s="46"/>
       <c r="S95" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="96" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="26">
         <v>2</v>
       </c>
@@ -10498,10 +10493,10 @@
       </c>
       <c r="R96" s="46"/>
       <c r="S96" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="97" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="26">
         <v>2</v>
       </c>
@@ -10555,10 +10550,10 @@
       </c>
       <c r="R97" s="46"/>
       <c r="S97" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="98" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="26">
         <v>2</v>
       </c>
@@ -10612,10 +10607,10 @@
       </c>
       <c r="R98" s="46"/>
       <c r="S98" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="99" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="26">
         <v>2</v>
       </c>
@@ -10669,10 +10664,10 @@
       </c>
       <c r="R99" s="46"/>
       <c r="S99" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="100" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="28">
         <v>2</v>
       </c>
@@ -10726,10 +10721,10 @@
       </c>
       <c r="R100" s="46"/>
       <c r="S100" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="101" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="28">
         <v>2</v>
       </c>
@@ -10783,10 +10778,10 @@
       </c>
       <c r="R101" s="46"/>
       <c r="S101" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="102" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="28">
         <v>2</v>
       </c>
@@ -10840,10 +10835,10 @@
       </c>
       <c r="R102" s="46"/>
       <c r="S102" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="103" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="29">
         <v>2</v>
       </c>
@@ -10897,7 +10892,7 @@
       </c>
       <c r="R103" s="46"/>
       <c r="S103" s="21" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="104" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11276,14 +11271,14 @@
         <v>1067</v>
       </c>
       <c r="P111" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q111" s="46">
         <v>44166</v>
       </c>
       <c r="R111" s="46"/>
       <c r="S111" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="112" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11333,7 +11328,7 @@
       <c r="R112" s="46"/>
       <c r="S112" s="21"/>
     </row>
-    <row r="113" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="29">
         <v>2</v>
       </c>
@@ -11387,7 +11382,7 @@
       </c>
       <c r="R113" s="46"/>
       <c r="S113" s="21" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="114" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11437,14 +11432,14 @@
         <v>1067</v>
       </c>
       <c r="P114" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q114" s="46">
         <v>44166</v>
       </c>
       <c r="R114" s="46"/>
       <c r="S114" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="115" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11494,14 +11489,14 @@
         <v>1067</v>
       </c>
       <c r="P115" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q115" s="46">
         <v>44166</v>
       </c>
       <c r="R115" s="46"/>
       <c r="S115" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="116" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11551,14 +11546,14 @@
         <v>1067</v>
       </c>
       <c r="P116" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q116" s="46">
         <v>44166</v>
       </c>
       <c r="R116" s="46"/>
       <c r="S116" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="117" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11702,14 +11697,14 @@
         <v>1067</v>
       </c>
       <c r="P119" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q119" s="46">
         <v>44166</v>
       </c>
       <c r="R119" s="46"/>
       <c r="S119" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="120" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11759,14 +11754,14 @@
         <v>1067</v>
       </c>
       <c r="P120" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q120" s="46">
         <v>44166</v>
       </c>
       <c r="R120" s="46"/>
       <c r="S120" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="121" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11816,14 +11811,14 @@
         <v>1067</v>
       </c>
       <c r="P121" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q121" s="46">
         <v>44166</v>
       </c>
       <c r="R121" s="46"/>
       <c r="S121" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="122" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11873,14 +11868,14 @@
         <v>1067</v>
       </c>
       <c r="P122" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q122" s="46">
         <v>44166</v>
       </c>
       <c r="R122" s="46"/>
       <c r="S122" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="123" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11930,14 +11925,14 @@
         <v>1067</v>
       </c>
       <c r="P123" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q123" s="46">
         <v>44166</v>
       </c>
       <c r="R123" s="46"/>
       <c r="S123" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="124" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -12034,17 +12029,17 @@
         <v>1067</v>
       </c>
       <c r="P125" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q125" s="46">
         <v>44166</v>
       </c>
       <c r="R125" s="46"/>
       <c r="S125" s="21" t="s">
-        <v>1239</v>
-      </c>
-    </row>
-    <row r="126" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="28">
         <v>2</v>
       </c>
@@ -12098,10 +12093,10 @@
       </c>
       <c r="R126" s="46"/>
       <c r="S126" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="127" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="28">
         <v>2</v>
       </c>
@@ -12155,10 +12150,10 @@
       </c>
       <c r="R127" s="46"/>
       <c r="S127" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="128" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="28">
         <v>2</v>
       </c>
@@ -12212,10 +12207,10 @@
       </c>
       <c r="R128" s="46"/>
       <c r="S128" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="129" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="28">
         <v>2</v>
       </c>
@@ -12269,10 +12264,10 @@
       </c>
       <c r="R129" s="46"/>
       <c r="S129" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="130" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="28">
         <v>2</v>
       </c>
@@ -12326,7 +12321,7 @@
       </c>
       <c r="R130" s="46"/>
       <c r="S130" s="21" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="131" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -12380,7 +12375,7 @@
       <c r="A132" s="28">
         <v>2</v>
       </c>
-      <c r="B132" s="26" t="s">
+      <c r="B132" s="15" t="s">
         <v>48</v>
       </c>
       <c r="C132" s="21" t="s">
@@ -12416,9 +12411,7 @@
       <c r="M132" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="N132" s="11" t="s">
-        <v>1217</v>
-      </c>
+      <c r="N132" s="11"/>
       <c r="O132" s="11" t="s">
         <v>1067</v>
       </c>
@@ -12474,7 +12467,7 @@
       <c r="R133" s="46"/>
       <c r="S133" s="21"/>
     </row>
-    <row r="134" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="28">
         <v>2</v>
       </c>
@@ -12528,10 +12521,10 @@
       </c>
       <c r="R134" s="46"/>
       <c r="S134" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="135" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="28">
         <v>2</v>
       </c>
@@ -12585,7 +12578,7 @@
       </c>
       <c r="R135" s="46"/>
       <c r="S135" s="21" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="136" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -12678,7 +12671,7 @@
       <c r="N137" s="12"/>
       <c r="O137" s="12"/>
       <c r="P137" s="21" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="Q137" s="46"/>
       <c r="R137" s="46"/>
@@ -12970,7 +12963,7 @@
       <c r="R143" s="46"/>
       <c r="S143" s="21"/>
     </row>
-    <row r="144" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="28">
         <v>2</v>
       </c>
@@ -13024,7 +13017,7 @@
       </c>
       <c r="R144" s="46"/>
       <c r="S144" s="21" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="145" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -13074,7 +13067,7 @@
       <c r="R145" s="46"/>
       <c r="S145" s="21"/>
     </row>
-    <row r="146" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="28">
         <v>2</v>
       </c>
@@ -13128,10 +13121,10 @@
       </c>
       <c r="R146" s="46"/>
       <c r="S146" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="147" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="28">
         <v>2</v>
       </c>
@@ -13185,10 +13178,10 @@
       </c>
       <c r="R147" s="46"/>
       <c r="S147" s="21" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="148" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="148" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="28">
         <v>2</v>
       </c>
@@ -13229,23 +13222,23 @@
         <v>25</v>
       </c>
       <c r="N148" s="11" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="O148" s="25" t="s">
         <v>1067</v>
       </c>
       <c r="P148" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q148" s="46">
         <v>44166</v>
       </c>
       <c r="R148" s="46"/>
       <c r="S148" s="21" t="s">
-        <v>1243</v>
-      </c>
-    </row>
-    <row r="149" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="28">
         <v>2</v>
       </c>
@@ -13286,23 +13279,23 @@
         <v>25</v>
       </c>
       <c r="N149" s="21" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="O149" s="25" t="s">
         <v>1067</v>
       </c>
       <c r="P149" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q149" s="46">
         <v>44166</v>
       </c>
       <c r="R149" s="46"/>
       <c r="S149" s="21" t="s">
-        <v>1243</v>
-      </c>
-    </row>
-    <row r="150" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="150" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="28">
         <v>2</v>
       </c>
@@ -13343,20 +13336,20 @@
         <v>25</v>
       </c>
       <c r="N150" s="21" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="O150" s="25" t="s">
         <v>1067</v>
       </c>
       <c r="P150" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q150" s="46">
         <v>44166</v>
       </c>
       <c r="R150" s="46"/>
       <c r="S150" s="21" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="151" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -13406,7 +13399,7 @@
       <c r="R151" s="46"/>
       <c r="S151" s="21"/>
     </row>
-    <row r="152" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="28">
         <v>2</v>
       </c>
@@ -13447,20 +13440,20 @@
         <v>25</v>
       </c>
       <c r="N152" s="21" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="O152" s="25" t="s">
         <v>1067</v>
       </c>
       <c r="P152" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q152" s="46">
         <v>44166</v>
       </c>
       <c r="R152" s="46"/>
       <c r="S152" s="21" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="153" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -13598,7 +13591,7 @@
         <v>25</v>
       </c>
       <c r="N155" s="21" t="s">
-        <v>1217</v>
+        <v>1250</v>
       </c>
       <c r="O155" s="25" t="s">
         <v>1067</v>
@@ -13649,7 +13642,7 @@
         <v>25</v>
       </c>
       <c r="N156" s="21" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="O156" s="25" t="s">
         <v>1067</v>
@@ -13700,7 +13693,7 @@
         <v>25</v>
       </c>
       <c r="N157" s="21" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="O157" s="25" t="s">
         <v>1067</v>
@@ -13756,7 +13749,7 @@
       <c r="R158" s="46"/>
       <c r="S158" s="21"/>
     </row>
-    <row r="159" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="32">
         <v>2</v>
       </c>
@@ -13797,7 +13790,7 @@
         <v>25</v>
       </c>
       <c r="N159" s="21" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="O159" s="25" t="s">
         <v>1067</v>
@@ -13901,7 +13894,7 @@
       <c r="R161" s="46"/>
       <c r="S161" s="21"/>
     </row>
-    <row r="162" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="32">
         <v>2</v>
       </c>
@@ -13955,7 +13948,7 @@
       </c>
       <c r="R162" s="46"/>
       <c r="S162" s="21" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="163" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -14099,7 +14092,7 @@
       <c r="R165" s="46"/>
       <c r="S165" s="21"/>
     </row>
-    <row r="166" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="27">
         <v>5</v>
       </c>
@@ -14139,24 +14132,24 @@
       <c r="M166" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="N166" s="11" t="s">
-        <v>1219</v>
+      <c r="N166" s="21" t="s">
+        <v>1218</v>
       </c>
       <c r="O166" s="25" t="s">
         <v>1067</v>
       </c>
       <c r="P166" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q166" s="46">
         <v>44166</v>
       </c>
       <c r="R166" s="46"/>
       <c r="S166" s="21" t="s">
-        <v>1243</v>
-      </c>
-    </row>
-    <row r="167" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="167" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="27">
         <v>5</v>
       </c>
@@ -14197,20 +14190,20 @@
         <v>25</v>
       </c>
       <c r="N167" s="21" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="O167" s="25" t="s">
         <v>1067</v>
       </c>
       <c r="P167" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q167" s="46">
         <v>44166</v>
       </c>
       <c r="R167" s="46"/>
       <c r="S167" s="21" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="168" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -14352,7 +14345,7 @@
         <v>25</v>
       </c>
       <c r="N170" s="11" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="O170" s="11" t="s">
         <v>1067</v>
@@ -14403,7 +14396,7 @@
         <v>25</v>
       </c>
       <c r="N171" s="21" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="O171" s="21" t="s">
         <v>1067</v>
@@ -14454,7 +14447,7 @@
         <v>25</v>
       </c>
       <c r="N172" s="21" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="O172" s="21" t="s">
         <v>1067</v>
@@ -14472,7 +14465,7 @@
         <v>558</v>
       </c>
       <c r="C173" s="21" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="D173" s="21" t="s">
         <v>503</v>
@@ -16720,14 +16713,14 @@
         <v>1067</v>
       </c>
       <c r="P220" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q220" s="46">
         <v>44166</v>
       </c>
       <c r="R220" s="46"/>
       <c r="S220" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="221" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -16818,20 +16811,20 @@
         <v>25</v>
       </c>
       <c r="N222" s="11" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O222" s="11" t="s">
         <v>1067</v>
       </c>
       <c r="P222" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q222" s="46">
         <v>44166</v>
       </c>
       <c r="R222" s="46"/>
       <c r="S222" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="223" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -16875,20 +16868,20 @@
         <v>26</v>
       </c>
       <c r="N223" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O223" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P223" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q223" s="46">
         <v>44166</v>
       </c>
       <c r="R223" s="46"/>
       <c r="S223" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="224" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -16932,20 +16925,20 @@
         <v>25</v>
       </c>
       <c r="N224" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O224" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P224" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q224" s="46">
         <v>44166</v>
       </c>
       <c r="R224" s="46"/>
       <c r="S224" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="225" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -16989,20 +16982,20 @@
         <v>26</v>
       </c>
       <c r="N225" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O225" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P225" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q225" s="46">
         <v>44166</v>
       </c>
       <c r="R225" s="46"/>
       <c r="S225" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="226" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17013,7 +17006,7 @@
         <v>284</v>
       </c>
       <c r="C226" s="21" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="D226" s="21" t="s">
         <v>462</v>
@@ -17046,20 +17039,20 @@
         <v>25</v>
       </c>
       <c r="N226" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O226" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P226" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q226" s="46">
         <v>44166</v>
       </c>
       <c r="R226" s="46"/>
       <c r="S226" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="227" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17103,20 +17096,20 @@
         <v>26</v>
       </c>
       <c r="N227" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O227" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P227" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q227" s="46">
         <v>44166</v>
       </c>
       <c r="R227" s="46"/>
       <c r="S227" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="228" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17160,20 +17153,20 @@
         <v>26</v>
       </c>
       <c r="N228" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O228" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P228" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q228" s="46">
         <v>44166</v>
       </c>
       <c r="R228" s="46"/>
       <c r="S228" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="229" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17217,20 +17210,20 @@
         <v>26</v>
       </c>
       <c r="N229" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O229" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P229" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q229" s="46">
         <v>44166</v>
       </c>
       <c r="R229" s="46"/>
       <c r="S229" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="230" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17274,20 +17267,20 @@
         <v>26</v>
       </c>
       <c r="N230" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O230" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P230" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q230" s="46">
         <v>44166</v>
       </c>
       <c r="R230" s="46"/>
       <c r="S230" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="231" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17331,20 +17324,20 @@
         <v>26</v>
       </c>
       <c r="N231" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O231" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P231" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q231" s="46">
         <v>44166</v>
       </c>
       <c r="R231" s="46"/>
       <c r="S231" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="232" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17388,20 +17381,20 @@
         <v>26</v>
       </c>
       <c r="N232" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O232" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P232" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q232" s="46">
         <v>44166</v>
       </c>
       <c r="R232" s="46"/>
       <c r="S232" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="233" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17445,20 +17438,20 @@
         <v>26</v>
       </c>
       <c r="N233" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O233" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P233" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q233" s="46">
         <v>44166</v>
       </c>
       <c r="R233" s="46"/>
       <c r="S233" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="234" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17502,20 +17495,20 @@
         <v>26</v>
       </c>
       <c r="N234" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O234" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P234" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q234" s="46">
         <v>44166</v>
       </c>
       <c r="R234" s="46"/>
       <c r="S234" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="235" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17559,20 +17552,20 @@
         <v>26</v>
       </c>
       <c r="N235" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O235" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P235" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q235" s="46">
         <v>44166</v>
       </c>
       <c r="R235" s="46"/>
       <c r="S235" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="236" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17616,20 +17609,20 @@
         <v>26</v>
       </c>
       <c r="N236" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O236" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P236" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q236" s="46">
         <v>44166</v>
       </c>
       <c r="R236" s="46"/>
       <c r="S236" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="237" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17673,20 +17666,20 @@
         <v>26</v>
       </c>
       <c r="N237" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O237" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P237" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q237" s="46">
         <v>44166</v>
       </c>
       <c r="R237" s="46"/>
       <c r="S237" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="238" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17730,20 +17723,20 @@
         <v>26</v>
       </c>
       <c r="N238" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O238" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P238" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q238" s="46">
         <v>44166</v>
       </c>
       <c r="R238" s="46"/>
       <c r="S238" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="239" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17787,20 +17780,20 @@
         <v>26</v>
       </c>
       <c r="N239" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O239" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P239" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q239" s="46">
         <v>44166</v>
       </c>
       <c r="R239" s="46"/>
       <c r="S239" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="240" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17844,20 +17837,20 @@
         <v>26</v>
       </c>
       <c r="N240" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O240" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P240" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q240" s="46">
         <v>44166</v>
       </c>
       <c r="R240" s="46"/>
       <c r="S240" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="241" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17901,20 +17894,20 @@
         <v>26</v>
       </c>
       <c r="N241" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O241" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P241" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q241" s="46">
         <v>44166</v>
       </c>
       <c r="R241" s="46"/>
       <c r="S241" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="242" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17958,20 +17951,20 @@
         <v>26</v>
       </c>
       <c r="N242" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O242" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P242" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q242" s="46">
         <v>44166</v>
       </c>
       <c r="R242" s="46"/>
       <c r="S242" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="243" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18015,20 +18008,20 @@
         <v>25</v>
       </c>
       <c r="N243" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O243" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P243" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q243" s="46">
         <v>44166</v>
       </c>
       <c r="R243" s="46"/>
       <c r="S243" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="244" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18072,20 +18065,20 @@
         <v>25</v>
       </c>
       <c r="N244" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O244" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P244" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q244" s="46">
         <v>44166</v>
       </c>
       <c r="R244" s="46"/>
       <c r="S244" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="245" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18129,20 +18122,20 @@
         <v>25</v>
       </c>
       <c r="N245" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O245" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P245" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q245" s="46">
         <v>44166</v>
       </c>
       <c r="R245" s="46"/>
       <c r="S245" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="246" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18186,20 +18179,20 @@
         <v>25</v>
       </c>
       <c r="N246" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O246" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P246" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q246" s="46">
         <v>44166</v>
       </c>
       <c r="R246" s="46"/>
       <c r="S246" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="247" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18243,20 +18236,20 @@
         <v>25</v>
       </c>
       <c r="N247" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O247" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P247" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q247" s="46">
         <v>44166</v>
       </c>
       <c r="R247" s="46"/>
       <c r="S247" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="248" spans="1:19" s="2" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18300,20 +18293,20 @@
         <v>25</v>
       </c>
       <c r="N248" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O248" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P248" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q248" s="46">
         <v>44166</v>
       </c>
       <c r="R248" s="46"/>
       <c r="S248" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="249" spans="1:19" s="2" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18357,20 +18350,20 @@
         <v>25</v>
       </c>
       <c r="N249" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O249" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P249" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q249" s="46">
         <v>44166</v>
       </c>
       <c r="R249" s="46"/>
       <c r="S249" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="250" spans="1:19" s="2" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18414,20 +18407,20 @@
         <v>25</v>
       </c>
       <c r="N250" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O250" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P250" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q250" s="46">
         <v>44166</v>
       </c>
       <c r="R250" s="46"/>
       <c r="S250" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="251" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18471,20 +18464,20 @@
         <v>26</v>
       </c>
       <c r="N251" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O251" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P251" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q251" s="46">
         <v>44166</v>
       </c>
       <c r="R251" s="46"/>
       <c r="S251" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="252" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18528,20 +18521,20 @@
         <v>26</v>
       </c>
       <c r="N252" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O252" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P252" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q252" s="46">
         <v>44166</v>
       </c>
       <c r="R252" s="46"/>
       <c r="S252" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="253" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18585,20 +18578,20 @@
         <v>26</v>
       </c>
       <c r="N253" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O253" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P253" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q253" s="46">
         <v>44166</v>
       </c>
       <c r="R253" s="46"/>
       <c r="S253" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="254" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18642,20 +18635,20 @@
         <v>26</v>
       </c>
       <c r="N254" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O254" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P254" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q254" s="46">
         <v>44166</v>
       </c>
       <c r="R254" s="46"/>
       <c r="S254" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="255" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18699,20 +18692,20 @@
         <v>26</v>
       </c>
       <c r="N255" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O255" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P255" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q255" s="46">
         <v>44166</v>
       </c>
       <c r="R255" s="46"/>
       <c r="S255" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="256" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18756,20 +18749,20 @@
         <v>26</v>
       </c>
       <c r="N256" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O256" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P256" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q256" s="46">
         <v>44166</v>
       </c>
       <c r="R256" s="46"/>
       <c r="S256" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="257" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18813,20 +18806,20 @@
         <v>25</v>
       </c>
       <c r="N257" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O257" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P257" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q257" s="46">
         <v>44166</v>
       </c>
       <c r="R257" s="46"/>
       <c r="S257" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="258" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18870,20 +18863,20 @@
         <v>26</v>
       </c>
       <c r="N258" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O258" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P258" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q258" s="46">
         <v>44166</v>
       </c>
       <c r="R258" s="46"/>
       <c r="S258" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="259" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18927,20 +18920,20 @@
         <v>26</v>
       </c>
       <c r="N259" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O259" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P259" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q259" s="46">
         <v>44166</v>
       </c>
       <c r="R259" s="46"/>
       <c r="S259" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="260" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -18984,20 +18977,20 @@
         <v>26</v>
       </c>
       <c r="N260" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O260" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P260" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q260" s="46">
         <v>44166</v>
       </c>
       <c r="R260" s="46"/>
       <c r="S260" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="261" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -19041,20 +19034,20 @@
         <v>25</v>
       </c>
       <c r="N261" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O261" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P261" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q261" s="46">
         <v>44166</v>
       </c>
       <c r="R261" s="46"/>
       <c r="S261" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="262" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -19098,20 +19091,20 @@
         <v>26</v>
       </c>
       <c r="N262" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O262" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P262" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q262" s="46">
         <v>44166</v>
       </c>
       <c r="R262" s="46"/>
       <c r="S262" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="263" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -19155,20 +19148,20 @@
         <v>26</v>
       </c>
       <c r="N263" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O263" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P263" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q263" s="46">
         <v>44166</v>
       </c>
       <c r="R263" s="46"/>
       <c r="S263" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="264" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -19212,20 +19205,20 @@
         <v>26</v>
       </c>
       <c r="N264" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O264" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P264" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q264" s="46">
         <v>44166</v>
       </c>
       <c r="R264" s="46"/>
       <c r="S264" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="265" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -19269,20 +19262,20 @@
         <v>26</v>
       </c>
       <c r="N265" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O265" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P265" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q265" s="46">
         <v>44166</v>
       </c>
       <c r="R265" s="46"/>
       <c r="S265" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="266" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -19326,20 +19319,20 @@
         <v>25</v>
       </c>
       <c r="N266" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O266" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P266" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q266" s="46">
         <v>44166</v>
       </c>
       <c r="R266" s="46"/>
       <c r="S266" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="267" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -19383,20 +19376,20 @@
         <v>25</v>
       </c>
       <c r="N267" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O267" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P267" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q267" s="46">
         <v>44166</v>
       </c>
       <c r="R267" s="46"/>
       <c r="S267" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="268" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -19407,7 +19400,7 @@
         <v>359</v>
       </c>
       <c r="C268" s="21" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="D268" s="21" t="s">
         <v>462</v>
@@ -19454,7 +19447,7 @@
         <v>360</v>
       </c>
       <c r="C269" s="21" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="D269" s="21" t="s">
         <v>462</v>
@@ -19640,20 +19633,20 @@
         <v>26</v>
       </c>
       <c r="N272" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O272" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P272" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q272" s="46">
         <v>44166</v>
       </c>
       <c r="R272" s="46"/>
       <c r="S272" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="273" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -19697,20 +19690,20 @@
         <v>26</v>
       </c>
       <c r="N273" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O273" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P273" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q273" s="46">
         <v>44166</v>
       </c>
       <c r="R273" s="46"/>
       <c r="S273" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="274" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -19848,20 +19841,20 @@
         <v>26</v>
       </c>
       <c r="N276" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O276" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P276" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q276" s="46">
         <v>44166</v>
       </c>
       <c r="R276" s="46"/>
       <c r="S276" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="277" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -19905,20 +19898,20 @@
         <v>26</v>
       </c>
       <c r="N277" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O277" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P277" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q277" s="46">
         <v>44166</v>
       </c>
       <c r="R277" s="46"/>
       <c r="S277" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="278" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -19962,20 +19955,20 @@
         <v>25</v>
       </c>
       <c r="N278" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O278" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P278" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q278" s="46">
         <v>44166</v>
       </c>
       <c r="R278" s="46"/>
       <c r="S278" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="279" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -20019,20 +20012,20 @@
         <v>25</v>
       </c>
       <c r="N279" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O279" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P279" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q279" s="46">
         <v>44166</v>
       </c>
       <c r="R279" s="46"/>
       <c r="S279" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="280" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -20264,20 +20257,20 @@
         <v>25</v>
       </c>
       <c r="N284" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O284" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P284" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q284" s="46">
         <v>44166</v>
       </c>
       <c r="R284" s="46"/>
       <c r="S284" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="285" spans="1:19" s="2" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -20462,20 +20455,20 @@
         <v>25</v>
       </c>
       <c r="N288" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O288" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P288" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q288" s="46">
         <v>44166</v>
       </c>
       <c r="R288" s="46"/>
       <c r="S288" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="289" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -20519,20 +20512,20 @@
         <v>25</v>
       </c>
       <c r="N289" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O289" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P289" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q289" s="46">
         <v>44166</v>
       </c>
       <c r="R289" s="46"/>
       <c r="S289" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="290" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -20576,20 +20569,20 @@
         <v>25</v>
       </c>
       <c r="N290" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O290" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P290" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q290" s="46">
         <v>44166</v>
       </c>
       <c r="R290" s="46"/>
       <c r="S290" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="291" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -20633,20 +20626,20 @@
         <v>25</v>
       </c>
       <c r="N291" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O291" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P291" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q291" s="46">
         <v>44166</v>
       </c>
       <c r="R291" s="46"/>
       <c r="S291" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="292" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -20690,20 +20683,20 @@
         <v>25</v>
       </c>
       <c r="N292" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O292" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P292" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q292" s="46">
         <v>44166</v>
       </c>
       <c r="R292" s="46"/>
       <c r="S292" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="293" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -20714,7 +20707,7 @@
         <v>617</v>
       </c>
       <c r="C293" s="21" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="D293" s="21" t="s">
         <v>462</v>
@@ -20747,20 +20740,20 @@
         <v>25</v>
       </c>
       <c r="N293" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O293" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P293" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q293" s="46">
         <v>44166</v>
       </c>
       <c r="R293" s="46"/>
       <c r="S293" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="294" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -20804,20 +20797,20 @@
         <v>25</v>
       </c>
       <c r="N294" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O294" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P294" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q294" s="46">
         <v>44166</v>
       </c>
       <c r="R294" s="46"/>
       <c r="S294" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="295" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -20912,20 +20905,20 @@
         <v>25</v>
       </c>
       <c r="N296" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O296" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P296" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q296" s="46">
         <v>44166</v>
       </c>
       <c r="R296" s="46"/>
       <c r="S296" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="297" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -21208,20 +21201,20 @@
         <v>25</v>
       </c>
       <c r="N302" s="11" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="O302" s="11" t="s">
         <v>1067</v>
       </c>
       <c r="P302" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q302" s="46">
         <v>44166</v>
       </c>
       <c r="R302" s="46"/>
       <c r="S302" s="21" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="303" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -21265,20 +21258,20 @@
         <v>25</v>
       </c>
       <c r="N303" s="11" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O303" s="11" t="s">
         <v>1067</v>
       </c>
       <c r="P303" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q303" s="46">
         <v>44166</v>
       </c>
       <c r="R303" s="46"/>
       <c r="S303" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="304" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -21322,20 +21315,20 @@
         <v>25</v>
       </c>
       <c r="N304" s="21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O304" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P304" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q304" s="46">
         <v>44166</v>
       </c>
       <c r="R304" s="46"/>
       <c r="S304" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="305" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -21379,20 +21372,20 @@
         <v>25</v>
       </c>
       <c r="N305" s="21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O305" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P305" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q305" s="46">
         <v>44166</v>
       </c>
       <c r="R305" s="46"/>
       <c r="S305" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="306" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -21906,20 +21899,20 @@
         <v>26</v>
       </c>
       <c r="N316" s="21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O316" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P316" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q316" s="46">
         <v>44166</v>
       </c>
       <c r="R316" s="46"/>
       <c r="S316" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="317" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -21963,20 +21956,20 @@
         <v>26</v>
       </c>
       <c r="N317" s="21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O317" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P317" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q317" s="46">
         <v>44166</v>
       </c>
       <c r="R317" s="46"/>
       <c r="S317" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="318" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22020,20 +22013,20 @@
         <v>26</v>
       </c>
       <c r="N318" s="21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O318" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P318" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q318" s="46">
         <v>44166</v>
       </c>
       <c r="R318" s="46"/>
       <c r="S318" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="319" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22077,20 +22070,20 @@
         <v>26</v>
       </c>
       <c r="N319" s="21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O319" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P319" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q319" s="46">
         <v>44166</v>
       </c>
       <c r="R319" s="46"/>
       <c r="S319" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="320" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22134,20 +22127,20 @@
         <v>26</v>
       </c>
       <c r="N320" s="21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O320" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P320" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q320" s="46">
         <v>44166</v>
       </c>
       <c r="R320" s="46"/>
       <c r="S320" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="321" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22285,20 +22278,20 @@
         <v>26</v>
       </c>
       <c r="N323" s="21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O323" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P323" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q323" s="46">
         <v>44166</v>
       </c>
       <c r="R323" s="46"/>
       <c r="S323" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="324" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22440,20 +22433,20 @@
         <v>26</v>
       </c>
       <c r="N326" s="11" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="O326" s="11" t="s">
         <v>1067</v>
       </c>
       <c r="P326" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q326" s="46">
         <v>44166</v>
       </c>
       <c r="R326" s="46"/>
       <c r="S326" s="21" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="327" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22497,20 +22490,20 @@
         <v>26</v>
       </c>
       <c r="N327" s="21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O327" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P327" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q327" s="46">
         <v>44166</v>
       </c>
       <c r="R327" s="46"/>
       <c r="S327" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="328" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22605,20 +22598,20 @@
         <v>25</v>
       </c>
       <c r="N329" s="21" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="O329" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P329" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q329" s="46">
         <v>44166</v>
       </c>
       <c r="R329" s="46"/>
       <c r="S329" s="21" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="330" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22662,20 +22655,20 @@
         <v>25</v>
       </c>
       <c r="N330" s="21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O330" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P330" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q330" s="46">
         <v>44166</v>
       </c>
       <c r="R330" s="46"/>
       <c r="S330" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="331" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22770,20 +22763,20 @@
         <v>25</v>
       </c>
       <c r="N332" s="21" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="O332" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P332" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q332" s="46">
         <v>44166</v>
       </c>
       <c r="R332" s="46"/>
       <c r="S332" s="21" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="333" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22827,20 +22820,20 @@
         <v>25</v>
       </c>
       <c r="N333" s="21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O333" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P333" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q333" s="46">
         <v>44166</v>
       </c>
       <c r="R333" s="46"/>
       <c r="S333" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="334" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22884,20 +22877,20 @@
         <v>25</v>
       </c>
       <c r="N334" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O334" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P334" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q334" s="46">
         <v>44166</v>
       </c>
       <c r="R334" s="46"/>
       <c r="S334" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="335" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22941,20 +22934,20 @@
         <v>25</v>
       </c>
       <c r="N335" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O335" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P335" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q335" s="46">
         <v>44166</v>
       </c>
       <c r="R335" s="46"/>
       <c r="S335" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="336" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -22998,20 +22991,20 @@
         <v>25</v>
       </c>
       <c r="N336" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O336" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P336" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q336" s="46">
         <v>44166</v>
       </c>
       <c r="R336" s="46"/>
       <c r="S336" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="337" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -31271,20 +31264,20 @@
         <v>85</v>
       </c>
       <c r="N513" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O513" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P513" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q513" s="46">
         <v>44166</v>
       </c>
       <c r="R513" s="46"/>
       <c r="S513" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="514" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -31328,20 +31321,20 @@
         <v>85</v>
       </c>
       <c r="N514" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O514" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P514" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q514" s="46">
         <v>44166</v>
       </c>
       <c r="R514" s="46"/>
       <c r="S514" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="515" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -31385,20 +31378,20 @@
         <v>85</v>
       </c>
       <c r="N515" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O515" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P515" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q515" s="46">
         <v>44166</v>
       </c>
       <c r="R515" s="46"/>
       <c r="S515" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="516" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -31442,20 +31435,20 @@
         <v>85</v>
       </c>
       <c r="N516" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O516" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P516" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q516" s="46">
         <v>44166</v>
       </c>
       <c r="R516" s="46"/>
       <c r="S516" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="517" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -31499,20 +31492,20 @@
         <v>85</v>
       </c>
       <c r="N517" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O517" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P517" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q517" s="46">
         <v>44166</v>
       </c>
       <c r="R517" s="46"/>
       <c r="S517" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="518" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -31556,20 +31549,20 @@
         <v>85</v>
       </c>
       <c r="N518" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O518" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P518" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q518" s="46">
         <v>44166</v>
       </c>
       <c r="R518" s="46"/>
       <c r="S518" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="519" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -31613,20 +31606,20 @@
         <v>85</v>
       </c>
       <c r="N519" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O519" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P519" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q519" s="46">
         <v>44166</v>
       </c>
       <c r="R519" s="46"/>
       <c r="S519" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="520" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -31670,20 +31663,20 @@
         <v>25</v>
       </c>
       <c r="N520" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O520" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P520" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q520" s="46">
         <v>44166</v>
       </c>
       <c r="R520" s="46"/>
       <c r="S520" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="521" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -31727,7 +31720,7 @@
         <v>85</v>
       </c>
       <c r="N521" s="11" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="O521" s="21" t="s">
         <v>1067</v>
@@ -31829,20 +31822,20 @@
         <v>26</v>
       </c>
       <c r="N523" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O523" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P523" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q523" s="46">
         <v>44166</v>
       </c>
       <c r="R523" s="46"/>
       <c r="S523" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="524" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -31886,20 +31879,20 @@
         <v>26</v>
       </c>
       <c r="N524" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O524" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P524" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q524" s="46">
         <v>44166</v>
       </c>
       <c r="R524" s="46"/>
       <c r="S524" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="525" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -31943,20 +31936,20 @@
         <v>85</v>
       </c>
       <c r="N525" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O525" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P525" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q525" s="46">
         <v>44166</v>
       </c>
       <c r="R525" s="46"/>
       <c r="S525" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="526" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -32000,20 +31993,20 @@
         <v>25</v>
       </c>
       <c r="N526" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O526" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P526" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q526" s="46">
         <v>44166</v>
       </c>
       <c r="R526" s="46"/>
       <c r="S526" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="527" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -32057,20 +32050,20 @@
         <v>25</v>
       </c>
       <c r="N527" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O527" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P527" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q527" s="46">
         <v>44166</v>
       </c>
       <c r="R527" s="46"/>
       <c r="S527" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="528" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -32114,20 +32107,20 @@
         <v>25</v>
       </c>
       <c r="N528" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O528" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P528" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q528" s="46">
         <v>44166</v>
       </c>
       <c r="R528" s="46"/>
       <c r="S528" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="529" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -32171,20 +32164,20 @@
         <v>25</v>
       </c>
       <c r="N529" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O529" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P529" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q529" s="46">
         <v>44166</v>
       </c>
       <c r="R529" s="46"/>
       <c r="S529" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="530" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -32228,20 +32221,20 @@
         <v>25</v>
       </c>
       <c r="N530" s="21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="O530" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P530" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q530" s="46">
         <v>44166</v>
       </c>
       <c r="R530" s="46"/>
       <c r="S530" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="531" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -32332,20 +32325,20 @@
         <v>25</v>
       </c>
       <c r="N532" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O532" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P532" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q532" s="46">
         <v>44166</v>
       </c>
       <c r="R532" s="46"/>
       <c r="S532" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="533" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -32389,20 +32382,20 @@
         <v>25</v>
       </c>
       <c r="N533" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O533" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P533" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q533" s="46">
         <v>44166</v>
       </c>
       <c r="R533" s="46"/>
       <c r="S533" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="534" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -32446,20 +32439,20 @@
         <v>25</v>
       </c>
       <c r="N534" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O534" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P534" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q534" s="46">
         <v>44166</v>
       </c>
       <c r="R534" s="46"/>
       <c r="S534" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="535" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -32503,20 +32496,20 @@
         <v>25</v>
       </c>
       <c r="N535" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O535" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P535" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q535" s="46">
         <v>44166</v>
       </c>
       <c r="R535" s="46"/>
       <c r="S535" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="536" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -32560,20 +32553,20 @@
         <v>25</v>
       </c>
       <c r="N536" s="21" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O536" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="P536" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q536" s="46">
         <v>44166</v>
       </c>
       <c r="R536" s="46"/>
       <c r="S536" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="537" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -32617,20 +32610,20 @@
         <v>25</v>
       </c>
       <c r="N537" s="25" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O537" s="25" t="s">
         <v>1067</v>
       </c>
       <c r="P537" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="Q537" s="46">
         <v>44166</v>
       </c>
       <c r="R537" s="46"/>
       <c r="S537" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="538" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -34898,7 +34891,7 @@
     </filterColumn>
     <filterColumn colId="13">
       <filters>
-        <filter val="opdracht_7"/>
+        <filter val="opdracht_11"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
omvang opdracht_13 van 57Mb naar 40Mb
</commit_message>
<xml_diff>
--- a/1.0.4-rc/Validatiematrix 1 (version 1).xlsb.xlsx
+++ b/1.0.4-rc/Validatiematrix 1 (version 1).xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_validatietestcontent\1.0.4-rc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7499B9DE-B283-4C61-ABAE-C2E6C0A23E50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1300BD3A-36D3-4B40-A75E-0C74B020C3E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="330" windowWidth="29040" windowHeight="15990" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5422,8 +5422,8 @@
   <dimension ref="A1:S585"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N148" sqref="N148"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6347,7 +6347,7 @@
       <c r="R19" s="46"/>
       <c r="S19" s="21"/>
     </row>
-    <row r="20" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="26">
         <v>4</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="26">
         <v>4</v>
       </c>
@@ -6461,7 +6461,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="26">
         <v>4</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="26">
         <v>4</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="26">
         <v>4</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26">
         <v>4</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27">
         <v>4</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="27">
         <v>4</v>
       </c>
@@ -6803,7 +6803,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="27">
         <v>4</v>
       </c>
@@ -6860,7 +6860,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27">
         <v>4</v>
       </c>
@@ -6917,7 +6917,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27">
         <v>4</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="27">
         <v>4</v>
       </c>
@@ -7031,7 +7031,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="27">
         <v>4</v>
       </c>
@@ -7088,7 +7088,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27">
         <v>4</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="27">
         <v>4</v>
       </c>
@@ -7194,7 +7194,7 @@
       <c r="R34" s="46"/>
       <c r="S34" s="21"/>
     </row>
-    <row r="35" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27">
         <v>4</v>
       </c>
@@ -7243,7 +7243,7 @@
       <c r="R35" s="46"/>
       <c r="S35" s="21"/>
     </row>
-    <row r="36" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27">
         <v>1</v>
       </c>
@@ -7294,7 +7294,7 @@
       <c r="R36" s="46"/>
       <c r="S36" s="21"/>
     </row>
-    <row r="37" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27">
         <v>1</v>
       </c>
@@ -7345,7 +7345,7 @@
       <c r="R37" s="46"/>
       <c r="S37" s="21"/>
     </row>
-    <row r="38" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="27">
         <v>1</v>
       </c>
@@ -7402,7 +7402,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="27">
         <v>1</v>
       </c>
@@ -7459,7 +7459,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="27">
         <v>1</v>
       </c>
@@ -7516,7 +7516,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="27">
         <v>1</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27">
         <v>1</v>
       </c>
@@ -7630,7 +7630,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="27">
         <v>1</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27">
         <v>1</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="27">
         <v>1</v>
       </c>
@@ -7801,7 +7801,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="27">
         <v>1</v>
       </c>
@@ -7860,7 +7860,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="27">
         <v>1</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="27">
         <v>1</v>
       </c>
@@ -7976,7 +7976,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="27">
         <v>1</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="27">
         <v>1</v>
       </c>
@@ -8094,7 +8094,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="27">
         <v>1</v>
       </c>
@@ -8151,7 +8151,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="27">
         <v>1</v>
       </c>
@@ -8208,7 +8208,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="27">
         <v>1</v>
       </c>
@@ -8265,7 +8265,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="27">
         <v>1</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="27">
         <v>1</v>
       </c>
@@ -8379,7 +8379,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27">
         <v>1</v>
       </c>
@@ -8436,7 +8436,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="26">
         <v>1</v>
       </c>
@@ -8748,7 +8748,7 @@
       <c r="R62" s="46"/>
       <c r="S62" s="21"/>
     </row>
-    <row r="63" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="28">
         <v>2</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="29">
         <v>2</v>
       </c>
@@ -8852,7 +8852,7 @@
       <c r="R64" s="46"/>
       <c r="S64" s="21"/>
     </row>
-    <row r="65" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="29">
         <v>2</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="29">
         <v>2</v>
       </c>
@@ -8960,7 +8960,7 @@
       <c r="R66" s="46"/>
       <c r="S66" s="21"/>
     </row>
-    <row r="67" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="29">
         <v>2</v>
       </c>
@@ -9011,7 +9011,7 @@
       <c r="R67" s="46"/>
       <c r="S67" s="21"/>
     </row>
-    <row r="68" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="29">
         <v>2</v>
       </c>
@@ -9062,7 +9062,7 @@
       <c r="R68" s="46"/>
       <c r="S68" s="21"/>
     </row>
-    <row r="69" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="29">
         <v>2</v>
       </c>
@@ -9109,7 +9109,7 @@
       <c r="R69" s="46"/>
       <c r="S69" s="21"/>
     </row>
-    <row r="70" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="29">
         <v>2</v>
       </c>
@@ -9156,7 +9156,7 @@
       <c r="R70" s="46"/>
       <c r="S70" s="21"/>
     </row>
-    <row r="71" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="29">
         <v>2</v>
       </c>
@@ -9207,7 +9207,7 @@
       <c r="R71" s="46"/>
       <c r="S71" s="21"/>
     </row>
-    <row r="72" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="29">
         <v>2</v>
       </c>
@@ -9258,7 +9258,7 @@
       <c r="R72" s="46"/>
       <c r="S72" s="21"/>
     </row>
-    <row r="73" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="29">
         <v>2</v>
       </c>
@@ -9305,7 +9305,7 @@
       <c r="R73" s="46"/>
       <c r="S73" s="21"/>
     </row>
-    <row r="74" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="30">
         <v>2</v>
       </c>
@@ -9352,7 +9352,7 @@
       <c r="R74" s="46"/>
       <c r="S74" s="21"/>
     </row>
-    <row r="75" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="29">
         <v>2</v>
       </c>
@@ -9409,7 +9409,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="29">
         <v>2</v>
       </c>
@@ -9456,7 +9456,7 @@
       <c r="R76" s="46"/>
       <c r="S76" s="21"/>
     </row>
-    <row r="77" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="29">
         <v>2</v>
       </c>
@@ -9503,7 +9503,7 @@
       <c r="R77" s="46"/>
       <c r="S77" s="21"/>
     </row>
-    <row r="78" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="29">
         <v>2</v>
       </c>
@@ -9550,7 +9550,7 @@
       <c r="R78" s="46"/>
       <c r="S78" s="21"/>
     </row>
-    <row r="79" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="29">
         <v>2</v>
       </c>
@@ -9597,7 +9597,7 @@
       <c r="R79" s="46"/>
       <c r="S79" s="21"/>
     </row>
-    <row r="80" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="29">
         <v>2</v>
       </c>
@@ -9644,7 +9644,7 @@
       <c r="R80" s="46"/>
       <c r="S80" s="21"/>
     </row>
-    <row r="81" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="29">
         <v>2</v>
       </c>
@@ -9691,7 +9691,7 @@
       <c r="R81" s="46"/>
       <c r="S81" s="21"/>
     </row>
-    <row r="82" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="29">
         <v>2</v>
       </c>
@@ -9738,7 +9738,7 @@
       <c r="R82" s="46"/>
       <c r="S82" s="21"/>
     </row>
-    <row r="83" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="29">
         <v>2</v>
       </c>
@@ -9785,7 +9785,7 @@
       <c r="R83" s="46"/>
       <c r="S83" s="21"/>
     </row>
-    <row r="84" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="29">
         <v>2</v>
       </c>
@@ -9834,7 +9834,7 @@
       <c r="R84" s="46"/>
       <c r="S84" s="21"/>
     </row>
-    <row r="85" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="28">
         <v>2</v>
       </c>
@@ -9881,7 +9881,7 @@
       <c r="R85" s="46"/>
       <c r="S85" s="21"/>
     </row>
-    <row r="86" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="28">
         <v>2</v>
       </c>
@@ -9938,7 +9938,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="28">
         <v>2</v>
       </c>
@@ -9985,7 +9985,7 @@
       <c r="R87" s="46"/>
       <c r="S87" s="21"/>
     </row>
-    <row r="88" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="26">
         <v>2</v>
       </c>
@@ -10042,7 +10042,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="26">
         <v>2</v>
       </c>
@@ -10099,7 +10099,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="26">
         <v>2</v>
       </c>
@@ -10156,7 +10156,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="26">
         <v>2</v>
       </c>
@@ -10213,7 +10213,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="26">
         <v>2</v>
       </c>
@@ -10270,7 +10270,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="26">
         <v>2</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="26">
         <v>2</v>
       </c>
@@ -10384,7 +10384,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="26">
         <v>2</v>
       </c>
@@ -10441,7 +10441,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="26">
         <v>2</v>
       </c>
@@ -10498,7 +10498,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="26">
         <v>2</v>
       </c>
@@ -10555,7 +10555,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="26">
         <v>2</v>
       </c>
@@ -10612,7 +10612,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="26">
         <v>2</v>
       </c>
@@ -10669,7 +10669,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="28">
         <v>2</v>
       </c>
@@ -10726,7 +10726,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="28">
         <v>2</v>
       </c>
@@ -10783,7 +10783,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="28">
         <v>2</v>
       </c>
@@ -10840,7 +10840,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="29">
         <v>2</v>
       </c>
@@ -10897,7 +10897,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="29">
         <v>2</v>
       </c>
@@ -10944,7 +10944,7 @@
       <c r="R104" s="46"/>
       <c r="S104" s="21"/>
     </row>
-    <row r="105" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="29">
         <v>2</v>
       </c>
@@ -10991,7 +10991,7 @@
       <c r="R105" s="46"/>
       <c r="S105" s="21"/>
     </row>
-    <row r="106" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="29">
         <v>2</v>
       </c>
@@ -11038,7 +11038,7 @@
       <c r="R106" s="46"/>
       <c r="S106" s="21"/>
     </row>
-    <row r="107" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="29">
         <v>2</v>
       </c>
@@ -11085,7 +11085,7 @@
       <c r="R107" s="46"/>
       <c r="S107" s="21"/>
     </row>
-    <row r="108" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="29">
         <v>2</v>
       </c>
@@ -11179,7 +11179,7 @@
       <c r="R109" s="46"/>
       <c r="S109" s="21"/>
     </row>
-    <row r="110" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="29">
         <v>2</v>
       </c>
@@ -11226,7 +11226,7 @@
       <c r="R110" s="46"/>
       <c r="S110" s="21"/>
     </row>
-    <row r="111" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="30">
         <v>2</v>
       </c>
@@ -11283,7 +11283,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="29">
         <v>2</v>
       </c>
@@ -11330,7 +11330,7 @@
       <c r="R112" s="46"/>
       <c r="S112" s="21"/>
     </row>
-    <row r="113" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="29">
         <v>2</v>
       </c>
@@ -11387,7 +11387,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="29">
         <v>2</v>
       </c>
@@ -11444,7 +11444,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="30">
         <v>2</v>
       </c>
@@ -11501,7 +11501,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="30">
         <v>2</v>
       </c>
@@ -11558,7 +11558,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="29">
         <v>2</v>
       </c>
@@ -11605,7 +11605,7 @@
       <c r="R117" s="46"/>
       <c r="S117" s="21"/>
     </row>
-    <row r="118" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="29">
         <v>2</v>
       </c>
@@ -11652,7 +11652,7 @@
       <c r="R118" s="46"/>
       <c r="S118" s="21"/>
     </row>
-    <row r="119" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="29">
         <v>2</v>
       </c>
@@ -11709,7 +11709,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="29">
         <v>2</v>
       </c>
@@ -11766,7 +11766,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="29">
         <v>2</v>
       </c>
@@ -11823,7 +11823,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="28">
         <v>2</v>
       </c>
@@ -11880,7 +11880,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="28">
         <v>2</v>
       </c>
@@ -11937,7 +11937,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="28">
         <v>2</v>
       </c>
@@ -11984,7 +11984,7 @@
       <c r="R124" s="46"/>
       <c r="S124" s="21"/>
     </row>
-    <row r="125" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="28">
         <v>2</v>
       </c>
@@ -12041,7 +12041,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="28">
         <v>2</v>
       </c>
@@ -12098,7 +12098,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="28">
         <v>2</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="28">
         <v>2</v>
       </c>
@@ -12212,7 +12212,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="28">
         <v>2</v>
       </c>
@@ -12269,7 +12269,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="28">
         <v>2</v>
       </c>
@@ -12326,7 +12326,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="28">
         <v>2</v>
       </c>
@@ -12373,7 +12373,7 @@
       <c r="R131" s="46"/>
       <c r="S131" s="21"/>
     </row>
-    <row r="132" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="28">
         <v>2</v>
       </c>
@@ -12422,7 +12422,7 @@
       <c r="R132" s="46"/>
       <c r="S132" s="21"/>
     </row>
-    <row r="133" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="28">
         <v>2</v>
       </c>
@@ -12469,7 +12469,7 @@
       <c r="R133" s="46"/>
       <c r="S133" s="21"/>
     </row>
-    <row r="134" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="28">
         <v>2</v>
       </c>
@@ -12526,7 +12526,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="28">
         <v>2</v>
       </c>
@@ -12583,7 +12583,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="28">
         <v>2</v>
       </c>
@@ -12630,7 +12630,7 @@
       <c r="R136" s="46"/>
       <c r="S136" s="21"/>
     </row>
-    <row r="137" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="28">
         <v>2</v>
       </c>
@@ -12679,7 +12679,7 @@
       <c r="R137" s="46"/>
       <c r="S137" s="21"/>
     </row>
-    <row r="138" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="26">
         <v>5</v>
       </c>
@@ -12726,7 +12726,7 @@
       <c r="R138" s="46"/>
       <c r="S138" s="21"/>
     </row>
-    <row r="139" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="26">
         <v>5</v>
       </c>
@@ -12820,7 +12820,7 @@
       <c r="R140" s="46"/>
       <c r="S140" s="21"/>
     </row>
-    <row r="141" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="26">
         <v>5</v>
       </c>
@@ -12871,7 +12871,7 @@
       <c r="R141" s="46"/>
       <c r="S141" s="21"/>
     </row>
-    <row r="142" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="26">
         <v>5</v>
       </c>
@@ -12965,7 +12965,7 @@
       <c r="R143" s="46"/>
       <c r="S143" s="21"/>
     </row>
-    <row r="144" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="28">
         <v>2</v>
       </c>
@@ -13022,7 +13022,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="28">
         <v>2</v>
       </c>
@@ -13069,7 +13069,7 @@
       <c r="R145" s="46"/>
       <c r="S145" s="21"/>
     </row>
-    <row r="146" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="28">
         <v>2</v>
       </c>
@@ -13126,7 +13126,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="28">
         <v>2</v>
       </c>
@@ -13354,7 +13354,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="28">
         <v>2</v>
       </c>
@@ -13458,7 +13458,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="28">
         <v>2</v>
       </c>
@@ -13505,7 +13505,7 @@
       <c r="R153" s="46"/>
       <c r="S153" s="21"/>
     </row>
-    <row r="154" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="28">
         <v>2</v>
       </c>
@@ -13552,7 +13552,7 @@
       <c r="R154" s="46"/>
       <c r="S154" s="21"/>
     </row>
-    <row r="155" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="28">
         <v>2</v>
       </c>
@@ -13603,7 +13603,7 @@
       <c r="R155" s="46"/>
       <c r="S155" s="21"/>
     </row>
-    <row r="156" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="28">
         <v>2</v>
       </c>
@@ -13654,7 +13654,7 @@
       <c r="R156" s="46"/>
       <c r="S156" s="21"/>
     </row>
-    <row r="157" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="32">
         <v>2</v>
       </c>
@@ -13705,7 +13705,7 @@
       <c r="R157" s="46"/>
       <c r="S157" s="21"/>
     </row>
-    <row r="158" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="32">
         <v>2</v>
       </c>
@@ -13802,7 +13802,7 @@
       <c r="R159" s="46"/>
       <c r="S159" s="21"/>
     </row>
-    <row r="160" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="28">
         <v>2</v>
       </c>
@@ -13849,7 +13849,7 @@
       <c r="R160" s="46"/>
       <c r="S160" s="21"/>
     </row>
-    <row r="161" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="32">
         <v>2</v>
       </c>
@@ -13896,7 +13896,7 @@
       <c r="R161" s="46"/>
       <c r="S161" s="21"/>
     </row>
-    <row r="162" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="32">
         <v>2</v>
       </c>
@@ -13953,7 +13953,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="32">
         <v>2</v>
       </c>
@@ -14047,7 +14047,7 @@
       <c r="R164" s="46"/>
       <c r="S164" s="21"/>
     </row>
-    <row r="165" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="27">
         <v>5</v>
       </c>
@@ -14208,7 +14208,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="27">
         <v>5</v>
       </c>
@@ -14259,7 +14259,7 @@
       <c r="R168" s="46"/>
       <c r="S168" s="21"/>
     </row>
-    <row r="169" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="27">
         <v>5</v>
       </c>
@@ -14306,7 +14306,7 @@
       <c r="R169" s="46"/>
       <c r="S169" s="21"/>
     </row>
-    <row r="170" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="26">
         <v>5</v>
       </c>
@@ -14357,7 +14357,7 @@
       <c r="R170" s="46"/>
       <c r="S170" s="21"/>
     </row>
-    <row r="171" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="27">
         <v>5</v>
       </c>
@@ -14408,7 +14408,7 @@
       <c r="R171" s="46"/>
       <c r="S171" s="21"/>
     </row>
-    <row r="172" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="27">
         <v>5</v>
       </c>
@@ -14459,7 +14459,7 @@
       <c r="R172" s="46"/>
       <c r="S172" s="21"/>
     </row>
-    <row r="173" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="27">
         <v>5</v>
       </c>
@@ -14506,7 +14506,7 @@
       <c r="R173" s="46"/>
       <c r="S173" s="21"/>
     </row>
-    <row r="174" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="27">
         <v>5</v>
       </c>
@@ -14553,7 +14553,7 @@
       <c r="R174" s="46"/>
       <c r="S174" s="21"/>
     </row>
-    <row r="175" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="27">
         <v>5</v>
       </c>
@@ -14600,7 +14600,7 @@
       <c r="R175" s="46"/>
       <c r="S175" s="21"/>
     </row>
-    <row r="176" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="27">
         <v>5</v>
       </c>
@@ -14647,7 +14647,7 @@
       <c r="R176" s="46"/>
       <c r="S176" s="21"/>
     </row>
-    <row r="177" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="27">
         <v>5</v>
       </c>
@@ -14694,7 +14694,7 @@
       <c r="R177" s="46"/>
       <c r="S177" s="21"/>
     </row>
-    <row r="178" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="27">
         <v>5</v>
       </c>
@@ -14741,7 +14741,7 @@
       <c r="R178" s="46"/>
       <c r="S178" s="21"/>
     </row>
-    <row r="179" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="27">
         <v>5</v>
       </c>
@@ -14788,7 +14788,7 @@
       <c r="R179" s="46"/>
       <c r="S179" s="21"/>
     </row>
-    <row r="180" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="27">
         <v>5</v>
       </c>
@@ -14835,7 +14835,7 @@
       <c r="R180" s="46"/>
       <c r="S180" s="21"/>
     </row>
-    <row r="181" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="27">
         <v>5</v>
       </c>
@@ -14882,7 +14882,7 @@
       <c r="R181" s="46"/>
       <c r="S181" s="21"/>
     </row>
-    <row r="182" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="27">
         <v>5</v>
       </c>
@@ -14929,7 +14929,7 @@
       <c r="R182" s="46"/>
       <c r="S182" s="21"/>
     </row>
-    <row r="183" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="27">
         <v>5</v>
       </c>
@@ -14976,7 +14976,7 @@
       <c r="R183" s="46"/>
       <c r="S183" s="21"/>
     </row>
-    <row r="184" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="27">
         <v>5</v>
       </c>
@@ -15023,7 +15023,7 @@
       <c r="R184" s="46"/>
       <c r="S184" s="21"/>
     </row>
-    <row r="185" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="27">
         <v>5</v>
       </c>
@@ -15070,7 +15070,7 @@
       <c r="R185" s="46"/>
       <c r="S185" s="21"/>
     </row>
-    <row r="186" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="27">
         <v>5</v>
       </c>
@@ -15117,7 +15117,7 @@
       <c r="R186" s="46"/>
       <c r="S186" s="21"/>
     </row>
-    <row r="187" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="27">
         <v>5</v>
       </c>
@@ -15164,7 +15164,7 @@
       <c r="R187" s="46"/>
       <c r="S187" s="21"/>
     </row>
-    <row r="188" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="27">
         <v>5</v>
       </c>
@@ -15211,7 +15211,7 @@
       <c r="R188" s="46"/>
       <c r="S188" s="21"/>
     </row>
-    <row r="189" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="27">
         <v>5</v>
       </c>
@@ -15258,7 +15258,7 @@
       <c r="R189" s="46"/>
       <c r="S189" s="21"/>
     </row>
-    <row r="190" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="27">
         <v>5</v>
       </c>
@@ -15305,7 +15305,7 @@
       <c r="R190" s="46"/>
       <c r="S190" s="21"/>
     </row>
-    <row r="191" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="27">
         <v>5</v>
       </c>
@@ -15352,7 +15352,7 @@
       <c r="R191" s="46"/>
       <c r="S191" s="21"/>
     </row>
-    <row r="192" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="27">
         <v>5</v>
       </c>
@@ -15399,7 +15399,7 @@
       <c r="R192" s="46"/>
       <c r="S192" s="21"/>
     </row>
-    <row r="193" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="27">
         <v>5</v>
       </c>
@@ -15446,7 +15446,7 @@
       <c r="R193" s="46"/>
       <c r="S193" s="21"/>
     </row>
-    <row r="194" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="27">
         <v>5</v>
       </c>
@@ -15493,7 +15493,7 @@
       <c r="R194" s="46"/>
       <c r="S194" s="21"/>
     </row>
-    <row r="195" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="27">
         <v>5</v>
       </c>
@@ -15540,7 +15540,7 @@
       <c r="R195" s="46"/>
       <c r="S195" s="21"/>
     </row>
-    <row r="196" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="27">
         <v>5</v>
       </c>
@@ -15587,7 +15587,7 @@
       <c r="R196" s="46"/>
       <c r="S196" s="21"/>
     </row>
-    <row r="197" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="27">
         <v>5</v>
       </c>
@@ -15634,7 +15634,7 @@
       <c r="R197" s="46"/>
       <c r="S197" s="21"/>
     </row>
-    <row r="198" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="27">
         <v>5</v>
       </c>
@@ -15681,7 +15681,7 @@
       <c r="R198" s="46"/>
       <c r="S198" s="21"/>
     </row>
-    <row r="199" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="27">
         <v>5</v>
       </c>
@@ -15728,7 +15728,7 @@
       <c r="R199" s="46"/>
       <c r="S199" s="21"/>
     </row>
-    <row r="200" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="27">
         <v>5</v>
       </c>
@@ -15775,7 +15775,7 @@
       <c r="R200" s="46"/>
       <c r="S200" s="21"/>
     </row>
-    <row r="201" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="27">
         <v>5</v>
       </c>
@@ -15822,7 +15822,7 @@
       <c r="R201" s="46"/>
       <c r="S201" s="21"/>
     </row>
-    <row r="202" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="27">
         <v>5</v>
       </c>
@@ -15869,7 +15869,7 @@
       <c r="R202" s="46"/>
       <c r="S202" s="21"/>
     </row>
-    <row r="203" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="27">
         <v>5</v>
       </c>
@@ -15916,7 +15916,7 @@
       <c r="R203" s="46"/>
       <c r="S203" s="21"/>
     </row>
-    <row r="204" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="27">
         <v>5</v>
       </c>
@@ -15963,7 +15963,7 @@
       <c r="R204" s="46"/>
       <c r="S204" s="21"/>
     </row>
-    <row r="205" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="27">
         <v>5</v>
       </c>
@@ -16010,7 +16010,7 @@
       <c r="R205" s="46"/>
       <c r="S205" s="21"/>
     </row>
-    <row r="206" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="27">
         <v>5</v>
       </c>
@@ -16057,7 +16057,7 @@
       <c r="R206" s="46"/>
       <c r="S206" s="21"/>
     </row>
-    <row r="207" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="27">
         <v>5</v>
       </c>
@@ -16104,7 +16104,7 @@
       <c r="R207" s="46"/>
       <c r="S207" s="21"/>
     </row>
-    <row r="208" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="27">
         <v>5</v>
       </c>
@@ -16151,7 +16151,7 @@
       <c r="R208" s="46"/>
       <c r="S208" s="21"/>
     </row>
-    <row r="209" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="27">
         <v>5</v>
       </c>
@@ -16198,7 +16198,7 @@
       <c r="R209" s="46"/>
       <c r="S209" s="21"/>
     </row>
-    <row r="210" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="27">
         <v>5</v>
       </c>
@@ -16245,7 +16245,7 @@
       <c r="R210" s="46"/>
       <c r="S210" s="21"/>
     </row>
-    <row r="211" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="27">
         <v>5</v>
       </c>
@@ -16292,7 +16292,7 @@
       <c r="R211" s="46"/>
       <c r="S211" s="21"/>
     </row>
-    <row r="212" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="27">
         <v>5</v>
       </c>
@@ -16339,7 +16339,7 @@
       <c r="R212" s="46"/>
       <c r="S212" s="21"/>
     </row>
-    <row r="213" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="27">
         <v>5</v>
       </c>
@@ -16386,7 +16386,7 @@
       <c r="R213" s="46"/>
       <c r="S213" s="21"/>
     </row>
-    <row r="214" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="27">
         <v>5</v>
       </c>
@@ -16433,7 +16433,7 @@
       <c r="R214" s="46"/>
       <c r="S214" s="21"/>
     </row>
-    <row r="215" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="27">
         <v>5</v>
       </c>
@@ -16480,7 +16480,7 @@
       <c r="R215" s="46"/>
       <c r="S215" s="21"/>
     </row>
-    <row r="216" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="27">
         <v>5</v>
       </c>
@@ -16527,7 +16527,7 @@
       <c r="R216" s="46"/>
       <c r="S216" s="21"/>
     </row>
-    <row r="217" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="27">
         <v>5</v>
       </c>
@@ -16574,7 +16574,7 @@
       <c r="R217" s="46"/>
       <c r="S217" s="21"/>
     </row>
-    <row r="218" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="27">
         <v>5</v>
       </c>
@@ -16621,7 +16621,7 @@
       <c r="R218" s="46"/>
       <c r="S218" s="21"/>
     </row>
-    <row r="219" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="27">
         <v>5</v>
       </c>
@@ -16668,7 +16668,7 @@
       <c r="R219" s="46"/>
       <c r="S219" s="21"/>
     </row>
-    <row r="220" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="27">
         <v>1</v>
       </c>
@@ -16725,7 +16725,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="27">
         <v>5</v>
       </c>
@@ -16772,7 +16772,7 @@
       <c r="R221" s="46"/>
       <c r="S221" s="21"/>
     </row>
-    <row r="222" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="29">
         <v>8</v>
       </c>
@@ -16829,7 +16829,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="29">
         <v>8</v>
       </c>
@@ -16886,7 +16886,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="224" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="29">
         <v>8</v>
       </c>
@@ -16943,7 +16943,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="225" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="29">
         <v>8</v>
       </c>
@@ -17000,7 +17000,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="226" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="29">
         <v>8</v>
       </c>
@@ -17057,7 +17057,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="227" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="29">
         <v>8</v>
       </c>
@@ -17114,7 +17114,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="228" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="29">
         <v>8</v>
       </c>
@@ -17171,7 +17171,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="229" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="29">
         <v>8</v>
       </c>
@@ -17228,7 +17228,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="230" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="29">
         <v>8</v>
       </c>
@@ -17285,7 +17285,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="231" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="29">
         <v>8</v>
       </c>
@@ -17342,7 +17342,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="232" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="29">
         <v>8</v>
       </c>
@@ -17399,7 +17399,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="233" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="29">
         <v>8</v>
       </c>
@@ -17456,7 +17456,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="234" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="29">
         <v>8</v>
       </c>
@@ -17513,7 +17513,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="235" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="29">
         <v>8</v>
       </c>
@@ -17570,7 +17570,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="236" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="29">
         <v>8</v>
       </c>
@@ -17627,7 +17627,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="237" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="29">
         <v>8</v>
       </c>
@@ -17684,7 +17684,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="238" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="29">
         <v>8</v>
       </c>
@@ -17741,7 +17741,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="29">
         <v>8</v>
       </c>
@@ -17798,7 +17798,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="240" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="29">
         <v>8</v>
       </c>
@@ -17855,7 +17855,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="241" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="29">
         <v>8</v>
       </c>
@@ -17912,7 +17912,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="242" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="29">
         <v>8</v>
       </c>
@@ -17969,7 +17969,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="243" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="29">
         <v>8</v>
       </c>
@@ -18026,7 +18026,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="244" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="29">
         <v>8</v>
       </c>
@@ -18083,7 +18083,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="245" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="29">
         <v>8</v>
       </c>
@@ -18140,7 +18140,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="246" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="29">
         <v>8</v>
       </c>
@@ -18197,7 +18197,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="247" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="29">
         <v>8</v>
       </c>
@@ -18254,7 +18254,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="248" spans="1:19" s="2" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:19" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="29">
         <v>8</v>
       </c>
@@ -18311,7 +18311,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="249" spans="1:19" s="2" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:19" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="29">
         <v>8</v>
       </c>
@@ -18368,7 +18368,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="250" spans="1:19" s="2" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:19" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="29">
         <v>8</v>
       </c>
@@ -18425,7 +18425,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="251" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="29">
         <v>8</v>
       </c>
@@ -18482,7 +18482,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="252" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="29">
         <v>8</v>
       </c>
@@ -18539,7 +18539,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="253" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="29">
         <v>8</v>
       </c>
@@ -18596,7 +18596,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="254" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="28">
         <v>8</v>
       </c>
@@ -18653,7 +18653,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="255" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="29">
         <v>8</v>
       </c>
@@ -18710,7 +18710,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="256" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="29">
         <v>8</v>
       </c>
@@ -18767,7 +18767,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="257" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="29">
         <v>8</v>
       </c>
@@ -18824,7 +18824,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="258" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="29">
         <v>8</v>
       </c>
@@ -18881,7 +18881,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="259" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="29">
         <v>8</v>
       </c>
@@ -18938,7 +18938,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="260" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="29">
         <v>8</v>
       </c>
@@ -18995,7 +18995,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="261" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="29">
         <v>8</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="262" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" s="29">
         <v>8</v>
       </c>
@@ -19109,7 +19109,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="263" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="29">
         <v>8</v>
       </c>
@@ -19166,7 +19166,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="264" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="28">
         <v>8</v>
       </c>
@@ -19223,7 +19223,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="265" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="29">
         <v>8</v>
       </c>
@@ -19280,7 +19280,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="266" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="29">
         <v>8</v>
       </c>
@@ -19337,7 +19337,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="267" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="29">
         <v>8</v>
       </c>
@@ -19394,7 +19394,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="268" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="29">
         <v>8</v>
       </c>
@@ -19441,7 +19441,7 @@
       <c r="R268" s="46"/>
       <c r="S268" s="21"/>
     </row>
-    <row r="269" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="29">
         <v>8</v>
       </c>
@@ -19492,7 +19492,7 @@
       <c r="R269" s="46"/>
       <c r="S269" s="21"/>
     </row>
-    <row r="270" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="29">
         <v>8</v>
       </c>
@@ -19543,7 +19543,7 @@
       <c r="R270" s="46"/>
       <c r="S270" s="21"/>
     </row>
-    <row r="271" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" s="29">
         <v>8</v>
       </c>
@@ -19594,7 +19594,7 @@
       <c r="R271" s="46"/>
       <c r="S271" s="21"/>
     </row>
-    <row r="272" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" s="29">
         <v>8</v>
       </c>
@@ -19651,7 +19651,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="273" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="29">
         <v>8</v>
       </c>
@@ -19708,7 +19708,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="274" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="29">
         <v>8</v>
       </c>
@@ -19755,7 +19755,7 @@
       <c r="R274" s="46"/>
       <c r="S274" s="21"/>
     </row>
-    <row r="275" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="29">
         <v>8</v>
       </c>
@@ -19802,7 +19802,7 @@
       <c r="R275" s="46"/>
       <c r="S275" s="21"/>
     </row>
-    <row r="276" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="29">
         <v>8</v>
       </c>
@@ -19859,7 +19859,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="277" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" s="29">
         <v>8</v>
       </c>
@@ -19916,7 +19916,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="278" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="29">
         <v>8</v>
       </c>
@@ -19973,7 +19973,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="279" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="29">
         <v>8</v>
       </c>
@@ -20124,7 +20124,7 @@
       <c r="R281" s="46"/>
       <c r="S281" s="21"/>
     </row>
-    <row r="282" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" s="29">
         <v>8</v>
       </c>
@@ -20171,7 +20171,7 @@
       <c r="R282" s="46"/>
       <c r="S282" s="21"/>
     </row>
-    <row r="283" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" s="29">
         <v>8</v>
       </c>
@@ -20218,7 +20218,7 @@
       <c r="R283" s="46"/>
       <c r="S283" s="21"/>
     </row>
-    <row r="284" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" s="29">
         <v>8</v>
       </c>
@@ -20322,7 +20322,7 @@
       <c r="R285" s="46"/>
       <c r="S285" s="21"/>
     </row>
-    <row r="286" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="29">
         <v>8</v>
       </c>
@@ -20369,7 +20369,7 @@
       <c r="R286" s="46"/>
       <c r="S286" s="21"/>
     </row>
-    <row r="287" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" s="29">
         <v>8</v>
       </c>
@@ -20416,7 +20416,7 @@
       <c r="R287" s="46"/>
       <c r="S287" s="21"/>
     </row>
-    <row r="288" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="29">
         <v>8</v>
       </c>
@@ -20473,7 +20473,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="289" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" s="29">
         <v>8</v>
       </c>
@@ -20530,7 +20530,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="290" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" s="29">
         <v>8</v>
       </c>
@@ -20587,7 +20587,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="291" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" s="29">
         <v>8</v>
       </c>
@@ -20644,7 +20644,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="292" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" s="29">
         <v>8</v>
       </c>
@@ -20701,7 +20701,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="293" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="29">
         <v>8</v>
       </c>
@@ -20758,7 +20758,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="294" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" s="29">
         <v>8</v>
       </c>
@@ -20815,7 +20815,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="295" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" s="29">
         <v>8</v>
       </c>
@@ -20866,7 +20866,7 @@
       <c r="R295" s="46"/>
       <c r="S295" s="21"/>
     </row>
-    <row r="296" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" s="27">
         <v>8</v>
       </c>
@@ -20923,7 +20923,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="297" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A297" s="29">
         <v>8</v>
       </c>
@@ -20970,7 +20970,7 @@
       <c r="R297" s="46"/>
       <c r="S297" s="21"/>
     </row>
-    <row r="298" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A298" s="29">
         <v>8</v>
       </c>
@@ -21017,7 +21017,7 @@
       <c r="R298" s="46"/>
       <c r="S298" s="21"/>
     </row>
-    <row r="299" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A299" s="29">
         <v>8</v>
       </c>
@@ -21064,7 +21064,7 @@
       <c r="R299" s="46"/>
       <c r="S299" s="21"/>
     </row>
-    <row r="300" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" s="29">
         <v>8</v>
       </c>
@@ -21276,7 +21276,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="304" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" s="29">
         <v>8</v>
       </c>
@@ -21333,7 +21333,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="305" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" s="29">
         <v>8</v>
       </c>
@@ -21390,7 +21390,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="306" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A306" s="29">
         <v>8</v>
       </c>
@@ -21437,7 +21437,7 @@
       <c r="R306" s="46"/>
       <c r="S306" s="21"/>
     </row>
-    <row r="307" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A307" s="29">
         <v>8</v>
       </c>
@@ -21484,7 +21484,7 @@
       <c r="R307" s="46"/>
       <c r="S307" s="21"/>
     </row>
-    <row r="308" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" s="29">
         <v>8</v>
       </c>
@@ -21531,7 +21531,7 @@
       <c r="R308" s="46"/>
       <c r="S308" s="21"/>
     </row>
-    <row r="309" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="29">
         <v>8</v>
       </c>
@@ -21625,7 +21625,7 @@
       <c r="R310" s="46"/>
       <c r="S310" s="21"/>
     </row>
-    <row r="311" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" s="29">
         <v>8</v>
       </c>
@@ -21672,7 +21672,7 @@
       <c r="R311" s="46"/>
       <c r="S311" s="21"/>
     </row>
-    <row r="312" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A312" s="29">
         <v>8</v>
       </c>
@@ -21719,7 +21719,7 @@
       <c r="R312" s="46"/>
       <c r="S312" s="21"/>
     </row>
-    <row r="313" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A313" s="29">
         <v>8</v>
       </c>
@@ -21766,7 +21766,7 @@
       <c r="R313" s="46"/>
       <c r="S313" s="21"/>
     </row>
-    <row r="314" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A314" s="29">
         <v>8</v>
       </c>
@@ -21813,7 +21813,7 @@
       <c r="R314" s="46"/>
       <c r="S314" s="21"/>
     </row>
-    <row r="315" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A315" s="29">
         <v>8</v>
       </c>
@@ -34889,12 +34889,6 @@
     <filterColumn colId="5">
       <filters>
         <filter val="Ja"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="13">
-      <filters>
-        <filter val="opdracht_11"/>
-        <filter val="opdracht_3"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -35711,18 +35705,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -35745,6 +35739,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{430E6B59-185B-464E-889D-EBB334F9461E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4AEB88-1F93-43C1-A78E-1A3EC40A664E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -35759,12 +35761,4 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{430E6B59-185B-464E-889D-EBB334F9461E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aanpassingen in de Excel gedaan.
</commit_message>
<xml_diff>
--- a/1.0.4-rc/Validatiematrix 1 (version 1).xlsb.xlsx
+++ b/1.0.4-rc/Validatiematrix 1 (version 1).xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicharddeGraaf\Desktop\Geonovum\4 - Voorbeeldbestanden\GITHub\xml_validatietestcontent\1.0.4-rc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2112F576-E80B-4584-AC25-D52E63C4C653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B368ACCD-2EFC-4CB1-9D40-C69A443457E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7939" uniqueCount="1267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7943" uniqueCount="1273">
   <si>
     <t>Is Opdracht.zip een geldige zip</t>
   </si>
@@ -3809,9 +3809,6 @@
     <t>(Geonovum) kijken hoe en wat.</t>
   </si>
   <si>
-    <t>Hoe is deze bedoeld?</t>
-  </si>
-  <si>
     <t>Actiehouder</t>
   </si>
   <si>
@@ -3851,9 +3848,6 @@
     <t>opdracht_lvbb1004</t>
   </si>
   <si>
-    <t>opdracht_lvbb1011</t>
-  </si>
-  <si>
     <t>opdracht_lvbb1022</t>
   </si>
   <si>
@@ -3888,6 +3882,30 @@
   </si>
   <si>
     <t>opdracht_lvbb1015.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1024.zip</t>
+  </si>
+  <si>
+    <t>Deze fout kan niet volgens OW-schema's, we krijgen LVBB1015 terug.</t>
+  </si>
+  <si>
+    <t>Geeft een LVBB1016-foutmelding</t>
+  </si>
+  <si>
+    <t>Kunnen we niet testen met OOW-portaal.</t>
+  </si>
+  <si>
+    <t>Hier komt een LVBB1021-fout terug ipv een LVBB-1011</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1011.zip</t>
+  </si>
+  <si>
+    <t>Geeft een LVBB1018-foutmelding</t>
+  </si>
+  <si>
+    <t>Geeft een LVBB1008-foutmelding, Test opnieuw draaien.</t>
   </si>
 </sst>
 </file>
@@ -4320,7 +4338,7 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4460,9 +4478,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4498,7 +4513,77 @@
     <cellStyle name="Standaard 8" xfId="6" xr:uid="{4492B760-AE1B-46F5-BB01-F20D2648A2DB}"/>
     <cellStyle name="Title 2" xfId="10" xr:uid="{7E65A99B-BE5B-4D5A-90AB-4BE5E71E069B}"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="73">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5122,10 +5207,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Project Timeline" pivot="0" count="4" xr9:uid="{94F838F7-CCC6-442C-9CDB-4977D3904284}">
-      <tableStyleElement type="wholeTable" dxfId="62"/>
-      <tableStyleElement type="headerRow" dxfId="61"/>
-      <tableStyleElement type="firstRowStripe" dxfId="60"/>
-      <tableStyleElement type="secondRowStripe" dxfId="59"/>
+      <tableStyleElement type="wholeTable" dxfId="72"/>
+      <tableStyleElement type="headerRow" dxfId="71"/>
+      <tableStyleElement type="firstRowStripe" dxfId="70"/>
+      <tableStyleElement type="secondRowStripe" dxfId="69"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -5493,9 +5578,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8557A4-2CF5-4E48-BD49-1C23F60C44EA}">
   <dimension ref="A1:S585"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N52" sqref="N52"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R56" sqref="R56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5511,7 +5596,7 @@
     <col min="15" max="15" width="5.28515625" customWidth="1"/>
     <col min="16" max="16" width="15.42578125" customWidth="1"/>
     <col min="17" max="18" width="11" style="44" customWidth="1"/>
-    <col min="19" max="19" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5567,7 +5652,7 @@
         <v>1231</v>
       </c>
       <c r="R1" s="45" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="S1" s="43" t="s">
         <v>1230</v>
@@ -6471,7 +6556,7 @@
       </c>
       <c r="R20" s="46"/>
       <c r="S20" s="21" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6525,7 +6610,7 @@
         <v>44166</v>
       </c>
       <c r="R21" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S21" s="21"/>
     </row>
@@ -6580,7 +6665,7 @@
         <v>44166</v>
       </c>
       <c r="R22" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S22" s="21"/>
     </row>
@@ -6635,7 +6720,7 @@
         <v>44166</v>
       </c>
       <c r="R23" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S23" s="21"/>
     </row>
@@ -6690,7 +6775,7 @@
         <v>44166</v>
       </c>
       <c r="R24" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S24" s="21"/>
     </row>
@@ -6745,7 +6830,7 @@
         <v>44166</v>
       </c>
       <c r="R25" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S25" s="21"/>
     </row>
@@ -6800,7 +6885,7 @@
         <v>44166</v>
       </c>
       <c r="R26" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S26" s="21"/>
     </row>
@@ -6855,7 +6940,7 @@
         <v>44166</v>
       </c>
       <c r="R27" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S27" s="21"/>
     </row>
@@ -6910,7 +6995,7 @@
         <v>44166</v>
       </c>
       <c r="R28" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S28" s="21"/>
     </row>
@@ -6965,7 +7050,7 @@
         <v>44166</v>
       </c>
       <c r="R29" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S29" s="21"/>
     </row>
@@ -7020,7 +7105,7 @@
         <v>44166</v>
       </c>
       <c r="R30" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S30" s="21"/>
     </row>
@@ -7075,7 +7160,7 @@
         <v>44166</v>
       </c>
       <c r="R31" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S31" s="21"/>
     </row>
@@ -7130,7 +7215,7 @@
         <v>44166</v>
       </c>
       <c r="R32" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S32" s="21"/>
     </row>
@@ -7185,7 +7270,7 @@
         <v>44166</v>
       </c>
       <c r="R33" s="46" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="S33" s="21"/>
     </row>
@@ -7443,7 +7528,7 @@
       </c>
       <c r="R38" s="46"/>
       <c r="S38" s="21" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7487,7 +7572,7 @@
         <v>24</v>
       </c>
       <c r="N39" s="11" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="O39" s="11" t="s">
         <v>1065</v>
@@ -7500,7 +7585,7 @@
       </c>
       <c r="R39" s="46"/>
       <c r="S39" s="21" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7544,7 +7629,7 @@
         <v>24</v>
       </c>
       <c r="N40" s="11" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="O40" s="11" t="s">
         <v>1065</v>
@@ -7557,7 +7642,7 @@
       </c>
       <c r="R40" s="46"/>
       <c r="S40" s="21" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7601,7 +7686,7 @@
         <v>24</v>
       </c>
       <c r="N41" s="11" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="O41" s="11" t="s">
         <v>1065</v>
@@ -7614,7 +7699,7 @@
       </c>
       <c r="R41" s="46"/>
       <c r="S41" s="21" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7658,7 +7743,7 @@
         <v>24</v>
       </c>
       <c r="N42" s="11" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="O42" s="11" t="s">
         <v>1065</v>
@@ -7671,7 +7756,7 @@
       </c>
       <c r="R42" s="46"/>
       <c r="S42" s="21" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7715,7 +7800,7 @@
         <v>24</v>
       </c>
       <c r="N43" s="11" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="O43" s="11" t="s">
         <v>1065</v>
@@ -7728,7 +7813,7 @@
       </c>
       <c r="R43" s="46"/>
       <c r="S43" s="21" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7772,7 +7857,7 @@
         <v>24</v>
       </c>
       <c r="N44" s="11" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="O44" s="11" t="s">
         <v>1065</v>
@@ -7785,7 +7870,7 @@
       </c>
       <c r="R44" s="46"/>
       <c r="S44" s="21" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7829,7 +7914,7 @@
         <v>24</v>
       </c>
       <c r="N45" s="11" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="O45" s="11" t="s">
         <v>1065</v>
@@ -7842,7 +7927,7 @@
       </c>
       <c r="R45" s="46"/>
       <c r="S45" s="21" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="46" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7853,7 +7938,7 @@
         <v>37</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="D46" s="21" t="s">
         <v>502</v>
@@ -7898,7 +7983,7 @@
         <v>44166</v>
       </c>
       <c r="R46" s="46" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="S46" s="21" t="s">
         <v>1233</v>
@@ -7957,7 +8042,7 @@
         <v>44166</v>
       </c>
       <c r="R47" s="46" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="S47" s="21" t="s">
         <v>1234</v>
@@ -8004,27 +8089,27 @@
         <v>24</v>
       </c>
       <c r="N48" s="11" t="s">
-        <v>1254</v>
+        <v>1270</v>
       </c>
       <c r="O48" s="11" t="s">
         <v>1065</v>
       </c>
-      <c r="P48" s="21">
-        <v>500</v>
+      <c r="P48" s="21" t="s">
+        <v>1232</v>
       </c>
       <c r="Q48" s="46">
-        <v>44167</v>
+        <v>44208</v>
       </c>
       <c r="R48" s="46"/>
       <c r="S48" s="21" t="s">
-        <v>1245</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="49" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
         <v>1</v>
       </c>
-      <c r="B49" s="47" t="s">
+      <c r="B49" s="39" t="s">
         <v>40</v>
       </c>
       <c r="C49" s="21" t="s">
@@ -8067,16 +8152,14 @@
         <v>1066</v>
       </c>
       <c r="P49" s="21" t="s">
-        <v>1232</v>
+        <v>84</v>
       </c>
       <c r="Q49" s="46">
-        <v>44166</v>
-      </c>
-      <c r="R49" s="46" t="s">
-        <v>1244</v>
-      </c>
+        <v>44208</v>
+      </c>
+      <c r="R49" s="46"/>
       <c r="S49" s="21" t="s">
-        <v>1240</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8120,7 +8203,7 @@
         <v>24</v>
       </c>
       <c r="N50" s="11" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="O50" s="11" t="s">
         <v>1066</v>
@@ -8133,7 +8216,7 @@
       </c>
       <c r="R50" s="46"/>
       <c r="S50" s="21" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8177,7 +8260,7 @@
         <v>24</v>
       </c>
       <c r="N51" s="11" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="O51" s="11" t="s">
         <v>1065</v>
@@ -8190,7 +8273,7 @@
       </c>
       <c r="R51" s="46"/>
       <c r="S51" s="21" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8240,14 +8323,14 @@
         <v>1066</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="Q52" s="46">
-        <v>44166</v>
+        <v>44208</v>
       </c>
       <c r="R52" s="46"/>
       <c r="S52" s="21" t="s">
-        <v>1235</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8300,11 +8383,13 @@
         <v>1232</v>
       </c>
       <c r="Q53" s="46">
-        <v>44166</v>
-      </c>
-      <c r="R53" s="46"/>
+        <v>44208</v>
+      </c>
+      <c r="R53" s="46" t="s">
+        <v>1241</v>
+      </c>
       <c r="S53" s="21" t="s">
-        <v>1235</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="54" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8354,14 +8439,14 @@
         <v>1066</v>
       </c>
       <c r="P54" s="21" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="Q54" s="46">
-        <v>44166</v>
+        <v>44208</v>
       </c>
       <c r="R54" s="46"/>
       <c r="S54" s="21" t="s">
-        <v>1235</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="55" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8411,12 +8496,14 @@
         <v>1066</v>
       </c>
       <c r="P55" s="21" t="s">
-        <v>1232</v>
+        <v>1256</v>
       </c>
       <c r="Q55" s="46">
-        <v>44166</v>
-      </c>
-      <c r="R55" s="46"/>
+        <v>44208</v>
+      </c>
+      <c r="R55" s="46" t="s">
+        <v>1243</v>
+      </c>
       <c r="S55" s="21" t="s">
         <v>1235</v>
       </c>
@@ -8467,15 +8554,13 @@
       <c r="O56" s="11" t="s">
         <v>1066</v>
       </c>
-      <c r="P56" s="21" t="s">
-        <v>1232</v>
-      </c>
+      <c r="P56" s="21"/>
       <c r="Q56" s="46">
-        <v>44166</v>
+        <v>44208</v>
       </c>
       <c r="R56" s="46"/>
       <c r="S56" s="21" t="s">
-        <v>1235</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="57" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8576,7 +8661,7 @@
         <v>24</v>
       </c>
       <c r="N58" s="21" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="O58" s="21" t="s">
         <v>1066</v>
@@ -8589,7 +8674,7 @@
       </c>
       <c r="R58" s="46"/>
       <c r="S58" s="21" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="59" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8633,7 +8718,7 @@
         <v>24</v>
       </c>
       <c r="N59" s="21" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="O59" s="21" t="s">
         <v>1066</v>
@@ -8646,7 +8731,7 @@
       </c>
       <c r="R59" s="46"/>
       <c r="S59" s="21" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="60" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8689,12 +8774,20 @@
       <c r="M60" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N60" s="11"/>
+      <c r="N60" s="11" t="s">
+        <v>1265</v>
+      </c>
       <c r="O60" s="11"/>
-      <c r="P60" s="21"/>
-      <c r="Q60" s="46"/>
+      <c r="P60" s="21" t="s">
+        <v>1232</v>
+      </c>
+      <c r="Q60" s="46">
+        <v>44208</v>
+      </c>
       <c r="R60" s="46"/>
-      <c r="S60" s="21"/>
+      <c r="S60" s="21" t="s">
+        <v>1266</v>
+      </c>
     </row>
     <row r="61" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="26">
@@ -8837,16 +8930,16 @@
         <v>1066</v>
       </c>
       <c r="P63" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q63" s="46">
         <v>44182</v>
       </c>
       <c r="R63" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S63" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="64" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8943,16 +9036,16 @@
         <v>1066</v>
       </c>
       <c r="P65" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q65" s="46">
         <v>44182</v>
       </c>
       <c r="R65" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S65" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="66" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9008,10 +9101,10 @@
         <v>44182</v>
       </c>
       <c r="R66" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S66" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="67" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9067,10 +9160,10 @@
         <v>44182</v>
       </c>
       <c r="R67" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S67" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9126,10 +9219,10 @@
         <v>44182</v>
       </c>
       <c r="R68" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S68" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9279,10 +9372,10 @@
         <v>44182</v>
       </c>
       <c r="R71" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S71" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="72" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9338,10 +9431,10 @@
         <v>44182</v>
       </c>
       <c r="R72" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S72" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="73" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9485,16 +9578,16 @@
         <v>1066</v>
       </c>
       <c r="P75" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q75" s="46">
         <v>44182</v>
       </c>
       <c r="R75" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S75" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="76" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10120,16 +10213,16 @@
         <v>1066</v>
       </c>
       <c r="P88" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q88" s="46">
         <v>44182</v>
       </c>
       <c r="R88" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S88" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="89" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10179,16 +10272,16 @@
         <v>1066</v>
       </c>
       <c r="P89" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q89" s="46">
         <v>44182</v>
       </c>
       <c r="R89" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S89" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="90" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10238,16 +10331,16 @@
         <v>1066</v>
       </c>
       <c r="P90" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q90" s="46">
         <v>44182</v>
       </c>
       <c r="R90" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S90" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="91" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10297,16 +10390,16 @@
         <v>1066</v>
       </c>
       <c r="P91" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q91" s="46">
         <v>44182</v>
       </c>
       <c r="R91" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S91" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="92" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10356,16 +10449,16 @@
         <v>1066</v>
       </c>
       <c r="P92" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q92" s="46">
         <v>44182</v>
       </c>
       <c r="R92" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S92" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="93" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10415,16 +10508,16 @@
         <v>1066</v>
       </c>
       <c r="P93" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q93" s="46">
         <v>44182</v>
       </c>
       <c r="R93" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S93" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="94" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10474,16 +10567,16 @@
         <v>1066</v>
       </c>
       <c r="P94" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q94" s="46">
         <v>44182</v>
       </c>
       <c r="R94" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S94" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="95" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10533,16 +10626,16 @@
         <v>1066</v>
       </c>
       <c r="P95" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q95" s="46">
         <v>44182</v>
       </c>
       <c r="R95" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S95" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="96" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10592,16 +10685,16 @@
         <v>1066</v>
       </c>
       <c r="P96" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q96" s="46">
         <v>44182</v>
       </c>
       <c r="R96" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S96" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="97" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10651,16 +10744,16 @@
         <v>1066</v>
       </c>
       <c r="P97" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q97" s="46">
         <v>44182</v>
       </c>
       <c r="R97" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S97" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="98" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10710,16 +10803,16 @@
         <v>1066</v>
       </c>
       <c r="P98" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q98" s="46">
         <v>44182</v>
       </c>
       <c r="R98" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S98" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="99" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10769,16 +10862,16 @@
         <v>1066</v>
       </c>
       <c r="P99" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q99" s="46">
         <v>44182</v>
       </c>
       <c r="R99" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S99" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="100" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10828,16 +10921,16 @@
         <v>1066</v>
       </c>
       <c r="P100" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q100" s="46">
         <v>44182</v>
       </c>
       <c r="R100" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S100" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="101" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10887,16 +10980,16 @@
         <v>1066</v>
       </c>
       <c r="P101" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q101" s="46">
         <v>44182</v>
       </c>
       <c r="R101" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S101" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="102" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10946,16 +11039,16 @@
         <v>1066</v>
       </c>
       <c r="P102" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q102" s="46">
         <v>44182</v>
       </c>
       <c r="R102" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S102" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="103" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11005,16 +11098,16 @@
         <v>1066</v>
       </c>
       <c r="P103" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q103" s="46">
         <v>44182</v>
       </c>
       <c r="R103" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S103" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="104" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11497,16 +11590,16 @@
         <v>1066</v>
       </c>
       <c r="P113" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q113" s="46">
         <v>44182</v>
       </c>
       <c r="R113" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S113" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="114" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12210,16 +12303,16 @@
         <v>1066</v>
       </c>
       <c r="P126" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q126" s="46">
         <v>44182</v>
       </c>
       <c r="R126" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S126" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="127" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12269,16 +12362,16 @@
         <v>1066</v>
       </c>
       <c r="P127" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q127" s="46">
         <v>44182</v>
       </c>
       <c r="R127" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S127" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="128" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12328,16 +12421,16 @@
         <v>1066</v>
       </c>
       <c r="P128" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q128" s="46">
         <v>44182</v>
       </c>
       <c r="R128" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S128" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="129" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12387,16 +12480,16 @@
         <v>1066</v>
       </c>
       <c r="P129" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q129" s="46">
         <v>44182</v>
       </c>
       <c r="R129" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S129" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="130" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12446,16 +12539,16 @@
         <v>1066</v>
       </c>
       <c r="P130" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q130" s="46">
         <v>44182</v>
       </c>
       <c r="R130" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S130" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="131" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12648,16 +12741,16 @@
         <v>1066</v>
       </c>
       <c r="P134" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q134" s="46">
         <v>44182</v>
       </c>
       <c r="R134" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S134" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="135" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12707,16 +12800,16 @@
         <v>1066</v>
       </c>
       <c r="P135" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q135" s="46">
         <v>44182</v>
       </c>
       <c r="R135" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S135" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="136" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13009,10 +13102,10 @@
         <v>44182</v>
       </c>
       <c r="R141" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S141" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="142" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13156,16 +13249,16 @@
         <v>1066</v>
       </c>
       <c r="P144" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q144" s="46">
         <v>44182</v>
       </c>
       <c r="R144" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S144" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="145" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13262,16 +13355,16 @@
         <v>1066</v>
       </c>
       <c r="P146" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q146" s="46">
         <v>44182</v>
       </c>
       <c r="R146" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S146" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="147" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13321,16 +13414,16 @@
         <v>1066</v>
       </c>
       <c r="P147" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q147" s="46">
         <v>44182</v>
       </c>
       <c r="R147" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S147" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="148" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13380,13 +13473,13 @@
         <v>1066</v>
       </c>
       <c r="P148" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q148" s="46">
         <v>44166</v>
       </c>
       <c r="R148" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S148" s="21" t="s">
         <v>1238</v>
@@ -13439,13 +13532,13 @@
         <v>1066</v>
       </c>
       <c r="P149" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q149" s="46">
         <v>44166</v>
       </c>
       <c r="R149" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S149" s="21" t="s">
         <v>1238</v>
@@ -13498,13 +13591,13 @@
         <v>1066</v>
       </c>
       <c r="P150" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q150" s="46">
         <v>44166</v>
       </c>
       <c r="R150" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S150" s="21" t="s">
         <v>1238</v>
@@ -13604,13 +13697,13 @@
         <v>1066</v>
       </c>
       <c r="P152" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q152" s="46">
         <v>44166</v>
       </c>
       <c r="R152" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S152" s="21" t="s">
         <v>1238</v>
@@ -13751,7 +13844,7 @@
         <v>24</v>
       </c>
       <c r="N155" s="21" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="O155" s="25" t="s">
         <v>1066</v>
@@ -13814,10 +13907,10 @@
         <v>44182</v>
       </c>
       <c r="R156" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S156" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="157" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13873,10 +13966,10 @@
         <v>44182</v>
       </c>
       <c r="R157" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S157" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="158" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13972,13 +14065,13 @@
         <v>1066</v>
       </c>
       <c r="P159" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q159" s="46">
         <v>44166</v>
       </c>
       <c r="R159" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S159" s="21" t="s">
         <v>1238</v>
@@ -14125,16 +14218,16 @@
         <v>1066</v>
       </c>
       <c r="P162" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q162" s="46">
         <v>44182</v>
       </c>
       <c r="R162" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S162" s="21" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="163" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14325,13 +14418,13 @@
         <v>1066</v>
       </c>
       <c r="P166" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q166" s="46">
         <v>44166</v>
       </c>
       <c r="R166" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S166" s="21" t="s">
         <v>1238</v>
@@ -14384,13 +14477,13 @@
         <v>1066</v>
       </c>
       <c r="P167" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q167" s="46">
         <v>44166</v>
       </c>
       <c r="R167" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S167" s="21" t="s">
         <v>1238</v>
@@ -14449,10 +14542,10 @@
         <v>44182</v>
       </c>
       <c r="R168" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S168" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="169" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14549,16 +14642,16 @@
         <v>1066</v>
       </c>
       <c r="P170" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q170" s="46">
         <v>44182</v>
       </c>
       <c r="R170" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S170" s="21" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="171" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14608,16 +14701,16 @@
         <v>1066</v>
       </c>
       <c r="P171" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q171" s="46">
         <v>44182</v>
       </c>
       <c r="R171" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S171" s="21" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="172" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14667,16 +14760,16 @@
         <v>1066</v>
       </c>
       <c r="P172" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q172" s="46">
         <v>44182</v>
       </c>
       <c r="R172" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S172" s="21" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="173" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16892,7 +16985,7 @@
       <c r="A220" s="27">
         <v>1</v>
       </c>
-      <c r="B220" s="48" t="s">
+      <c r="B220" s="47" t="s">
         <v>790</v>
       </c>
       <c r="C220" s="21" t="s">
@@ -17039,7 +17132,7 @@
         <v>1066</v>
       </c>
       <c r="P222" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q222" s="46">
         <v>44166</v>
@@ -17096,7 +17189,7 @@
         <v>1066</v>
       </c>
       <c r="P223" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q223" s="46">
         <v>44166</v>
@@ -17153,7 +17246,7 @@
         <v>1066</v>
       </c>
       <c r="P224" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q224" s="46">
         <v>44166</v>
@@ -17210,7 +17303,7 @@
         <v>1066</v>
       </c>
       <c r="P225" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q225" s="46">
         <v>44166</v>
@@ -17267,7 +17360,7 @@
         <v>1066</v>
       </c>
       <c r="P226" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q226" s="46">
         <v>44166</v>
@@ -17324,7 +17417,7 @@
         <v>1066</v>
       </c>
       <c r="P227" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q227" s="46">
         <v>44166</v>
@@ -17381,7 +17474,7 @@
         <v>1066</v>
       </c>
       <c r="P228" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q228" s="46">
         <v>44166</v>
@@ -17438,7 +17531,7 @@
         <v>1066</v>
       </c>
       <c r="P229" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q229" s="46">
         <v>44166</v>
@@ -17495,7 +17588,7 @@
         <v>1066</v>
       </c>
       <c r="P230" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q230" s="46">
         <v>44166</v>
@@ -17552,7 +17645,7 @@
         <v>1066</v>
       </c>
       <c r="P231" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q231" s="46">
         <v>44166</v>
@@ -17609,7 +17702,7 @@
         <v>1066</v>
       </c>
       <c r="P232" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q232" s="46">
         <v>44166</v>
@@ -17666,7 +17759,7 @@
         <v>1066</v>
       </c>
       <c r="P233" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q233" s="46">
         <v>44166</v>
@@ -17723,7 +17816,7 @@
         <v>1066</v>
       </c>
       <c r="P234" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q234" s="46">
         <v>44166</v>
@@ -17780,7 +17873,7 @@
         <v>1066</v>
       </c>
       <c r="P235" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q235" s="46">
         <v>44166</v>
@@ -17837,7 +17930,7 @@
         <v>1066</v>
       </c>
       <c r="P236" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q236" s="46">
         <v>44166</v>
@@ -17894,7 +17987,7 @@
         <v>1066</v>
       </c>
       <c r="P237" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q237" s="46">
         <v>44166</v>
@@ -17951,7 +18044,7 @@
         <v>1066</v>
       </c>
       <c r="P238" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q238" s="46">
         <v>44166</v>
@@ -18008,7 +18101,7 @@
         <v>1066</v>
       </c>
       <c r="P239" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q239" s="46">
         <v>44166</v>
@@ -18065,7 +18158,7 @@
         <v>1066</v>
       </c>
       <c r="P240" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q240" s="46">
         <v>44166</v>
@@ -18122,7 +18215,7 @@
         <v>1066</v>
       </c>
       <c r="P241" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q241" s="46">
         <v>44166</v>
@@ -18179,7 +18272,7 @@
         <v>1066</v>
       </c>
       <c r="P242" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q242" s="46">
         <v>44166</v>
@@ -18236,7 +18329,7 @@
         <v>1066</v>
       </c>
       <c r="P243" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q243" s="46">
         <v>44166</v>
@@ -18293,7 +18386,7 @@
         <v>1066</v>
       </c>
       <c r="P244" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q244" s="46">
         <v>44166</v>
@@ -18350,7 +18443,7 @@
         <v>1066</v>
       </c>
       <c r="P245" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q245" s="46">
         <v>44166</v>
@@ -18407,7 +18500,7 @@
         <v>1066</v>
       </c>
       <c r="P246" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q246" s="46">
         <v>44166</v>
@@ -18464,7 +18557,7 @@
         <v>1066</v>
       </c>
       <c r="P247" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q247" s="46">
         <v>44166</v>
@@ -18521,7 +18614,7 @@
         <v>1066</v>
       </c>
       <c r="P248" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q248" s="46">
         <v>44166</v>
@@ -18578,7 +18671,7 @@
         <v>1066</v>
       </c>
       <c r="P249" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q249" s="46">
         <v>44166</v>
@@ -18635,7 +18728,7 @@
         <v>1066</v>
       </c>
       <c r="P250" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q250" s="46">
         <v>44166</v>
@@ -18692,7 +18785,7 @@
         <v>1066</v>
       </c>
       <c r="P251" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q251" s="46">
         <v>44166</v>
@@ -18749,7 +18842,7 @@
         <v>1066</v>
       </c>
       <c r="P252" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q252" s="46">
         <v>44166</v>
@@ -18806,7 +18899,7 @@
         <v>1066</v>
       </c>
       <c r="P253" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q253" s="46">
         <v>44166</v>
@@ -18863,7 +18956,7 @@
         <v>1066</v>
       </c>
       <c r="P254" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q254" s="46">
         <v>44166</v>
@@ -18920,7 +19013,7 @@
         <v>1066</v>
       </c>
       <c r="P255" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q255" s="46">
         <v>44166</v>
@@ -18977,7 +19070,7 @@
         <v>1066</v>
       </c>
       <c r="P256" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q256" s="46">
         <v>44166</v>
@@ -19034,7 +19127,7 @@
         <v>1066</v>
       </c>
       <c r="P257" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q257" s="46">
         <v>44166</v>
@@ -19091,7 +19184,7 @@
         <v>1066</v>
       </c>
       <c r="P258" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q258" s="46">
         <v>44166</v>
@@ -19148,7 +19241,7 @@
         <v>1066</v>
       </c>
       <c r="P259" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q259" s="46">
         <v>44166</v>
@@ -19205,7 +19298,7 @@
         <v>1066</v>
       </c>
       <c r="P260" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q260" s="46">
         <v>44166</v>
@@ -19262,7 +19355,7 @@
         <v>1066</v>
       </c>
       <c r="P261" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q261" s="46">
         <v>44166</v>
@@ -19319,7 +19412,7 @@
         <v>1066</v>
       </c>
       <c r="P262" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q262" s="46">
         <v>44166</v>
@@ -19376,7 +19469,7 @@
         <v>1066</v>
       </c>
       <c r="P263" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q263" s="46">
         <v>44166</v>
@@ -19433,7 +19526,7 @@
         <v>1066</v>
       </c>
       <c r="P264" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q264" s="46">
         <v>44166</v>
@@ -19490,7 +19583,7 @@
         <v>1066</v>
       </c>
       <c r="P265" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q265" s="46">
         <v>44166</v>
@@ -19547,7 +19640,7 @@
         <v>1066</v>
       </c>
       <c r="P266" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q266" s="46">
         <v>44166</v>
@@ -19604,7 +19697,7 @@
         <v>1066</v>
       </c>
       <c r="P267" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q267" s="46">
         <v>44166</v>
@@ -19714,10 +19807,10 @@
         <v>44182</v>
       </c>
       <c r="R269" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S269" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="270" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19773,10 +19866,10 @@
         <v>44182</v>
       </c>
       <c r="R270" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S270" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="271" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19832,10 +19925,10 @@
         <v>44182</v>
       </c>
       <c r="R271" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S271" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="272" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19885,7 +19978,7 @@
         <v>1066</v>
       </c>
       <c r="P272" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q272" s="46">
         <v>44166</v>
@@ -19942,7 +20035,7 @@
         <v>1066</v>
       </c>
       <c r="P273" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q273" s="46">
         <v>44166</v>
@@ -20093,7 +20186,7 @@
         <v>1066</v>
       </c>
       <c r="P276" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q276" s="46">
         <v>44166</v>
@@ -20150,7 +20243,7 @@
         <v>1066</v>
       </c>
       <c r="P277" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q277" s="46">
         <v>44166</v>
@@ -20207,7 +20300,7 @@
         <v>1066</v>
       </c>
       <c r="P278" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q278" s="46">
         <v>44166</v>
@@ -20264,7 +20357,7 @@
         <v>1066</v>
       </c>
       <c r="P279" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q279" s="46">
         <v>44166</v>
@@ -20509,7 +20602,7 @@
         <v>1066</v>
       </c>
       <c r="P284" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q284" s="46">
         <v>44166</v>
@@ -20707,7 +20800,7 @@
         <v>1066</v>
       </c>
       <c r="P288" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q288" s="46">
         <v>44166</v>
@@ -20764,7 +20857,7 @@
         <v>1066</v>
       </c>
       <c r="P289" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q289" s="46">
         <v>44166</v>
@@ -20821,7 +20914,7 @@
         <v>1066</v>
       </c>
       <c r="P290" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q290" s="46">
         <v>44166</v>
@@ -20878,7 +20971,7 @@
         <v>1066</v>
       </c>
       <c r="P291" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q291" s="46">
         <v>44166</v>
@@ -20935,7 +21028,7 @@
         <v>1066</v>
       </c>
       <c r="P292" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q292" s="46">
         <v>44166</v>
@@ -20992,7 +21085,7 @@
         <v>1066</v>
       </c>
       <c r="P293" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q293" s="46">
         <v>44166</v>
@@ -21049,7 +21142,7 @@
         <v>1066</v>
       </c>
       <c r="P294" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q294" s="46">
         <v>44166</v>
@@ -21112,10 +21205,10 @@
         <v>44182</v>
       </c>
       <c r="R295" s="46" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="S295" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="296" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21165,7 +21258,7 @@
         <v>1066</v>
       </c>
       <c r="P296" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q296" s="46">
         <v>44166</v>
@@ -21575,7 +21668,7 @@
         <v>1066</v>
       </c>
       <c r="P304" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q304" s="46">
         <v>44182</v>
@@ -21632,7 +21725,7 @@
         <v>1066</v>
       </c>
       <c r="P305" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="Q305" s="46">
         <v>44182</v>
@@ -35140,11 +35233,22 @@
   <autoFilter ref="A1:S585" xr:uid="{462B357B-D08B-41C7-9173-012688EAF9F7}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"NOK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"TestAanpassen"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"nvt"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P54">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"nvt"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35186,10 +35290,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="48"/>
       <c r="C1" s="6" t="s">
         <v>60</v>
       </c>
@@ -35474,12 +35578,12 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1 C1 A2:C37 A39:C1048576">
-    <cfRule type="containsText" dxfId="58" priority="31" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="68" priority="31" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:C38">
-    <cfRule type="containsText" dxfId="57" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="67" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A38)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Excel bijgewerkt n.a.v. uitgevoerde tests.
</commit_message>
<xml_diff>
--- a/1.0.4-rc/Validatiematrix 1 (version 1).xlsb.xlsx
+++ b/1.0.4-rc/Validatiematrix 1 (version 1).xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicharddeGraaf\Desktop\Geonovum\4 - Voorbeeldbestanden\GITHub\xml_validatietestcontent\1.0.4-rc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B368ACCD-2EFC-4CB1-9D40-C69A443457E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF85CE2-C0DB-4417-8A11-7212555E9437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7943" uniqueCount="1273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7984" uniqueCount="1287">
   <si>
     <t>Is Opdracht.zip een geldige zip</t>
   </si>
@@ -3788,12 +3788,6 @@
     <t>NOK</t>
   </si>
   <si>
-    <t>bestaat_niet.xml geeft geen fout terug?</t>
-  </si>
-  <si>
-    <t>zit_niet_in_manifest.xml geeft geen fout (?)</t>
-  </si>
-  <si>
     <t>Nog uitzoeken wat hier gebeurd is.</t>
   </si>
   <si>
@@ -3821,39 +3815,9 @@
     <t>Geonovum</t>
   </si>
   <si>
-    <t>Internal Server Error</t>
-  </si>
-  <si>
     <t>opdracht_17</t>
   </si>
   <si>
-    <t>opdracht_lvbb1002</t>
-  </si>
-  <si>
-    <t>opdracht_lvbb1003</t>
-  </si>
-  <si>
-    <t>opdracht_lvbb1005</t>
-  </si>
-  <si>
-    <t>opdracht_lvbb1006</t>
-  </si>
-  <si>
-    <t>opdracht_lvbb1007</t>
-  </si>
-  <si>
-    <t>opdracht_lvbb1008</t>
-  </si>
-  <si>
-    <t>opdracht_lvbb1004</t>
-  </si>
-  <si>
-    <t>opdracht_lvbb1022</t>
-  </si>
-  <si>
-    <t>opdracht_lvbb1023</t>
-  </si>
-  <si>
     <t>De enige fout die getriggerd wordt is LVBB1010</t>
   </si>
   <si>
@@ -3872,9 +3836,6 @@
     <t>DatumBekendmaking ligt in het verleden</t>
   </si>
   <si>
-    <t>We krijgen hier een andere fout terug (1018, die onterecht is.)</t>
-  </si>
-  <si>
     <t>opdracht_lvbb1013.zip</t>
   </si>
   <si>
@@ -3887,7 +3848,10 @@
     <t>opdracht_lvbb1024.zip</t>
   </si>
   <si>
-    <t>Deze fout kan niet volgens OW-schema's, we krijgen LVBB1015 terug.</t>
+    <t>opdracht_lvbb1025.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1026.zip</t>
   </si>
   <si>
     <t>Geeft een LVBB1016-foutmelding</t>
@@ -3896,16 +3860,94 @@
     <t>Kunnen we niet testen met OOW-portaal.</t>
   </si>
   <si>
-    <t>Hier komt een LVBB1021-fout terug ipv een LVBB-1011</t>
-  </si>
-  <si>
     <t>opdracht_lvbb1011.zip</t>
   </si>
   <si>
     <t>Geeft een LVBB1018-foutmelding</t>
   </si>
   <si>
-    <t>Geeft een LVBB1008-foutmelding, Test opnieuw draaien.</t>
+    <t>Geeft een LVBB1019-foutmelding</t>
+  </si>
+  <si>
+    <t>Geeft een LVBB1512-foutmelding</t>
+  </si>
+  <si>
+    <t>Geeft een LVBB1010-foutmelding</t>
+  </si>
+  <si>
+    <t>Geeft een LVBB1015-foutmelding (kan ook niet volgens OW-schema's).</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1016.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1017.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1018.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1019.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1020.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1021.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1022.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1023.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1002.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1003.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1004.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1005.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1006.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1007.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1008.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1009.zip</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1010.zip</t>
+  </si>
+  <si>
+    <t>Geeft een LVBB1021-foutmelding</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1501.zip</t>
+  </si>
+  <si>
+    <t>Geeft een LVBB1006-foutmelding</t>
+  </si>
+  <si>
+    <t>opdracht_lvbb1503.zip</t>
+  </si>
+  <si>
+    <t>We weten niet wat hier exact gevalideerd wordt.</t>
+  </si>
+  <si>
+    <t>Maken zodra wijzigingsbesluiten überhaupt kunnen.</t>
+  </si>
+  <si>
+    <t>Test moet nog gemaakt worden.</t>
   </si>
 </sst>
 </file>
@@ -4513,7 +4555,7 @@
     <cellStyle name="Standaard 8" xfId="6" xr:uid="{4492B760-AE1B-46F5-BB01-F20D2648A2DB}"/>
     <cellStyle name="Title 2" xfId="10" xr:uid="{7E65A99B-BE5B-4D5A-90AB-4BE5E71E069B}"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -4546,590 +4588,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5207,10 +4665,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Project Timeline" pivot="0" count="4" xr9:uid="{94F838F7-CCC6-442C-9CDB-4977D3904284}">
-      <tableStyleElement type="wholeTable" dxfId="72"/>
-      <tableStyleElement type="headerRow" dxfId="71"/>
-      <tableStyleElement type="firstRowStripe" dxfId="70"/>
-      <tableStyleElement type="secondRowStripe" dxfId="69"/>
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="firstRowStripe" dxfId="8"/>
+      <tableStyleElement type="secondRowStripe" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -5578,9 +5036,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8557A4-2CF5-4E48-BD49-1C23F60C44EA}">
   <dimension ref="A1:S585"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R56" sqref="R56"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5652,7 +5110,7 @@
         <v>1231</v>
       </c>
       <c r="R1" s="45" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="S1" s="43" t="s">
         <v>1230</v>
@@ -6556,7 +6014,7 @@
       </c>
       <c r="R20" s="46"/>
       <c r="S20" s="21" t="s">
-        <v>1260</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6610,7 +6068,7 @@
         <v>44166</v>
       </c>
       <c r="R21" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S21" s="21"/>
     </row>
@@ -6665,7 +6123,7 @@
         <v>44166</v>
       </c>
       <c r="R22" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S22" s="21"/>
     </row>
@@ -6720,7 +6178,7 @@
         <v>44166</v>
       </c>
       <c r="R23" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S23" s="21"/>
     </row>
@@ -6775,7 +6233,7 @@
         <v>44166</v>
       </c>
       <c r="R24" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S24" s="21"/>
     </row>
@@ -6830,7 +6288,7 @@
         <v>44166</v>
       </c>
       <c r="R25" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S25" s="21"/>
     </row>
@@ -6885,7 +6343,7 @@
         <v>44166</v>
       </c>
       <c r="R26" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S26" s="21"/>
     </row>
@@ -6940,7 +6398,7 @@
         <v>44166</v>
       </c>
       <c r="R27" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S27" s="21"/>
     </row>
@@ -6995,7 +6453,7 @@
         <v>44166</v>
       </c>
       <c r="R28" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S28" s="21"/>
     </row>
@@ -7050,7 +6508,7 @@
         <v>44166</v>
       </c>
       <c r="R29" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S29" s="21"/>
     </row>
@@ -7105,7 +6563,7 @@
         <v>44166</v>
       </c>
       <c r="R30" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S30" s="21"/>
     </row>
@@ -7160,7 +6618,7 @@
         <v>44166</v>
       </c>
       <c r="R31" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S31" s="21"/>
     </row>
@@ -7215,7 +6673,7 @@
         <v>44166</v>
       </c>
       <c r="R32" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S32" s="21"/>
     </row>
@@ -7270,7 +6728,7 @@
         <v>44166</v>
       </c>
       <c r="R33" s="46" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="S33" s="21"/>
     </row>
@@ -7515,20 +6973,20 @@
         <v>24</v>
       </c>
       <c r="N38" s="11" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="O38" s="11" t="s">
         <v>1065</v>
       </c>
-      <c r="P38" s="21">
-        <v>500</v>
-      </c>
-      <c r="Q38" s="46">
-        <v>44167</v>
-      </c>
-      <c r="R38" s="46"/>
+      <c r="P38" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q38" s="46"/>
+      <c r="R38" s="46" t="s">
+        <v>1241</v>
+      </c>
       <c r="S38" s="21" t="s">
-        <v>1244</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7572,20 +7030,22 @@
         <v>24</v>
       </c>
       <c r="N39" s="11" t="s">
-        <v>1246</v>
+        <v>1271</v>
       </c>
       <c r="O39" s="11" t="s">
         <v>1065</v>
       </c>
-      <c r="P39" s="21">
-        <v>500</v>
+      <c r="P39" s="21" t="s">
+        <v>84</v>
       </c>
       <c r="Q39" s="46">
-        <v>44167</v>
-      </c>
-      <c r="R39" s="46"/>
+        <v>44208</v>
+      </c>
+      <c r="R39" s="46" t="s">
+        <v>1241</v>
+      </c>
       <c r="S39" s="21" t="s">
-        <v>1244</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7629,20 +7089,22 @@
         <v>24</v>
       </c>
       <c r="N40" s="11" t="s">
-        <v>1247</v>
+        <v>1272</v>
       </c>
       <c r="O40" s="11" t="s">
         <v>1065</v>
       </c>
-      <c r="P40" s="21">
-        <v>500</v>
+      <c r="P40" s="21" t="s">
+        <v>84</v>
       </c>
       <c r="Q40" s="46">
-        <v>44167</v>
-      </c>
-      <c r="R40" s="46"/>
+        <v>44208</v>
+      </c>
+      <c r="R40" s="46" t="s">
+        <v>1241</v>
+      </c>
       <c r="S40" s="21" t="s">
-        <v>1244</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7686,20 +7148,22 @@
         <v>24</v>
       </c>
       <c r="N41" s="11" t="s">
-        <v>1252</v>
+        <v>1273</v>
       </c>
       <c r="O41" s="11" t="s">
         <v>1065</v>
       </c>
-      <c r="P41" s="21">
-        <v>500</v>
+      <c r="P41" s="21" t="s">
+        <v>84</v>
       </c>
       <c r="Q41" s="46">
-        <v>44167</v>
-      </c>
-      <c r="R41" s="46"/>
+        <v>44208</v>
+      </c>
+      <c r="R41" s="46" t="s">
+        <v>1241</v>
+      </c>
       <c r="S41" s="21" t="s">
-        <v>1244</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7743,20 +7207,22 @@
         <v>24</v>
       </c>
       <c r="N42" s="11" t="s">
-        <v>1248</v>
+        <v>1274</v>
       </c>
       <c r="O42" s="11" t="s">
         <v>1065</v>
       </c>
-      <c r="P42" s="21">
-        <v>500</v>
+      <c r="P42" s="21" t="s">
+        <v>84</v>
       </c>
       <c r="Q42" s="46">
-        <v>44167</v>
-      </c>
-      <c r="R42" s="46"/>
+        <v>44208</v>
+      </c>
+      <c r="R42" s="46" t="s">
+        <v>1241</v>
+      </c>
       <c r="S42" s="21" t="s">
-        <v>1244</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7800,20 +7266,22 @@
         <v>24</v>
       </c>
       <c r="N43" s="11" t="s">
-        <v>1249</v>
+        <v>1275</v>
       </c>
       <c r="O43" s="11" t="s">
         <v>1065</v>
       </c>
-      <c r="P43" s="21">
-        <v>500</v>
+      <c r="P43" s="21" t="s">
+        <v>84</v>
       </c>
       <c r="Q43" s="46">
-        <v>44167</v>
-      </c>
-      <c r="R43" s="46"/>
+        <v>44208</v>
+      </c>
+      <c r="R43" s="46" t="s">
+        <v>1241</v>
+      </c>
       <c r="S43" s="21" t="s">
-        <v>1244</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7857,20 +7325,22 @@
         <v>24</v>
       </c>
       <c r="N44" s="11" t="s">
-        <v>1250</v>
+        <v>1276</v>
       </c>
       <c r="O44" s="11" t="s">
         <v>1065</v>
       </c>
-      <c r="P44" s="21">
-        <v>500</v>
+      <c r="P44" s="21" t="s">
+        <v>84</v>
       </c>
       <c r="Q44" s="46">
-        <v>44167</v>
-      </c>
-      <c r="R44" s="46"/>
+        <v>44208</v>
+      </c>
+      <c r="R44" s="46" t="s">
+        <v>1241</v>
+      </c>
       <c r="S44" s="21" t="s">
-        <v>1244</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7914,20 +7384,22 @@
         <v>24</v>
       </c>
       <c r="N45" s="11" t="s">
-        <v>1251</v>
+        <v>1277</v>
       </c>
       <c r="O45" s="11" t="s">
         <v>1065</v>
       </c>
-      <c r="P45" s="21">
-        <v>500</v>
+      <c r="P45" s="21" t="s">
+        <v>84</v>
       </c>
       <c r="Q45" s="46">
-        <v>44167</v>
-      </c>
-      <c r="R45" s="46"/>
+        <v>44208</v>
+      </c>
+      <c r="R45" s="46" t="s">
+        <v>1241</v>
+      </c>
       <c r="S45" s="21" t="s">
-        <v>1244</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="46" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7938,7 +7410,7 @@
         <v>37</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>1259</v>
+        <v>1247</v>
       </c>
       <c r="D46" s="21" t="s">
         <v>502</v>
@@ -7971,7 +7443,7 @@
         <v>24</v>
       </c>
       <c r="N46" s="11" t="s">
-        <v>1211</v>
+        <v>1278</v>
       </c>
       <c r="O46" s="11" t="s">
         <v>1066</v>
@@ -7980,13 +7452,13 @@
         <v>1232</v>
       </c>
       <c r="Q46" s="46">
-        <v>44166</v>
+        <v>44208</v>
       </c>
       <c r="R46" s="46" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="S46" s="21" t="s">
-        <v>1233</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8030,22 +7502,20 @@
         <v>24</v>
       </c>
       <c r="N47" s="11" t="s">
-        <v>1211</v>
+        <v>1279</v>
       </c>
       <c r="O47" s="11" t="s">
         <v>1066</v>
       </c>
       <c r="P47" s="21" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="Q47" s="46">
-        <v>44166</v>
-      </c>
-      <c r="R47" s="46" t="s">
-        <v>1241</v>
-      </c>
+        <v>44208</v>
+      </c>
+      <c r="R47" s="46"/>
       <c r="S47" s="21" t="s">
-        <v>1234</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8089,7 +7559,7 @@
         <v>24</v>
       </c>
       <c r="N48" s="11" t="s">
-        <v>1270</v>
+        <v>1257</v>
       </c>
       <c r="O48" s="11" t="s">
         <v>1065</v>
@@ -8100,9 +7570,11 @@
       <c r="Q48" s="46">
         <v>44208</v>
       </c>
-      <c r="R48" s="46"/>
+      <c r="R48" s="46" t="s">
+        <v>1239</v>
+      </c>
       <c r="S48" s="21" t="s">
-        <v>1269</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="49" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8159,7 +7631,7 @@
       </c>
       <c r="R49" s="46"/>
       <c r="S49" s="21" t="s">
-        <v>1268</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8203,7 +7675,7 @@
         <v>24</v>
       </c>
       <c r="N50" s="11" t="s">
-        <v>1262</v>
+        <v>1249</v>
       </c>
       <c r="O50" s="11" t="s">
         <v>1066</v>
@@ -8214,9 +7686,11 @@
       <c r="Q50" s="46">
         <v>44208</v>
       </c>
-      <c r="R50" s="46"/>
+      <c r="R50" s="46" t="s">
+        <v>1239</v>
+      </c>
       <c r="S50" s="21" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8260,7 +7734,7 @@
         <v>24</v>
       </c>
       <c r="N51" s="11" t="s">
-        <v>1264</v>
+        <v>1251</v>
       </c>
       <c r="O51" s="11" t="s">
         <v>1065</v>
@@ -8273,7 +7747,7 @@
       </c>
       <c r="R51" s="46"/>
       <c r="S51" s="21" t="s">
-        <v>1263</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8316,8 +7790,8 @@
       <c r="M52" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N52" s="11" t="s">
-        <v>1211</v>
+      <c r="N52" s="21" t="s">
+        <v>1263</v>
       </c>
       <c r="O52" s="11" t="s">
         <v>1066</v>
@@ -8330,7 +7804,7 @@
       </c>
       <c r="R52" s="46"/>
       <c r="S52" s="21" t="s">
-        <v>1267</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8373,8 +7847,8 @@
       <c r="M53" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N53" s="11" t="s">
-        <v>1211</v>
+      <c r="N53" s="21" t="s">
+        <v>1264</v>
       </c>
       <c r="O53" s="11" t="s">
         <v>1066</v>
@@ -8386,10 +7860,10 @@
         <v>44208</v>
       </c>
       <c r="R53" s="46" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="S53" s="21" t="s">
-        <v>1271</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="54" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8432,8 +7906,8 @@
       <c r="M54" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N54" s="11" t="s">
-        <v>1211</v>
+      <c r="N54" s="21" t="s">
+        <v>1265</v>
       </c>
       <c r="O54" s="11" t="s">
         <v>1066</v>
@@ -8446,7 +7920,7 @@
       </c>
       <c r="R54" s="46"/>
       <c r="S54" s="21" t="s">
-        <v>1271</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="55" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8489,23 +7963,23 @@
       <c r="M55" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N55" s="11" t="s">
-        <v>1211</v>
+      <c r="N55" s="21" t="s">
+        <v>1266</v>
       </c>
       <c r="O55" s="11" t="s">
         <v>1066</v>
       </c>
       <c r="P55" s="21" t="s">
-        <v>1256</v>
+        <v>1229</v>
       </c>
       <c r="Q55" s="46">
         <v>44208</v>
       </c>
       <c r="R55" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S55" s="21" t="s">
-        <v>1235</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="56" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8548,19 +8022,23 @@
       <c r="M56" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N56" s="11" t="s">
-        <v>1211</v>
+      <c r="N56" s="21" t="s">
+        <v>1267</v>
       </c>
       <c r="O56" s="11" t="s">
         <v>1066</v>
       </c>
-      <c r="P56" s="21"/>
+      <c r="P56" s="21" t="s">
+        <v>1232</v>
+      </c>
       <c r="Q56" s="46">
         <v>44208</v>
       </c>
-      <c r="R56" s="46"/>
+      <c r="R56" s="46" t="s">
+        <v>1239</v>
+      </c>
       <c r="S56" s="21" t="s">
-        <v>1272</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="57" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8603,8 +8081,8 @@
       <c r="M57" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N57" s="11" t="s">
-        <v>1211</v>
+      <c r="N57" s="21" t="s">
+        <v>1268</v>
       </c>
       <c r="O57" s="11" t="s">
         <v>1066</v>
@@ -8613,11 +8091,13 @@
         <v>1232</v>
       </c>
       <c r="Q57" s="46">
-        <v>44166</v>
-      </c>
-      <c r="R57" s="46"/>
+        <v>44208</v>
+      </c>
+      <c r="R57" s="46" t="s">
+        <v>1239</v>
+      </c>
       <c r="S57" s="21" t="s">
-        <v>1235</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="58" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8661,20 +8141,20 @@
         <v>24</v>
       </c>
       <c r="N58" s="21" t="s">
-        <v>1253</v>
+        <v>1269</v>
       </c>
       <c r="O58" s="21" t="s">
         <v>1066</v>
       </c>
-      <c r="P58" s="21">
-        <v>500</v>
+      <c r="P58" s="21" t="s">
+        <v>84</v>
       </c>
       <c r="Q58" s="46">
-        <v>44167</v>
+        <v>44208</v>
       </c>
       <c r="R58" s="46"/>
       <c r="S58" s="21" t="s">
-        <v>1244</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="59" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8718,20 +8198,20 @@
         <v>24</v>
       </c>
       <c r="N59" s="21" t="s">
-        <v>1254</v>
+        <v>1270</v>
       </c>
       <c r="O59" s="21" t="s">
         <v>1066</v>
       </c>
-      <c r="P59" s="21">
-        <v>500</v>
+      <c r="P59" s="21" t="s">
+        <v>84</v>
       </c>
       <c r="Q59" s="46">
-        <v>44167</v>
+        <v>44208</v>
       </c>
       <c r="R59" s="46"/>
       <c r="S59" s="21" t="s">
-        <v>1244</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="60" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8775,7 +8255,7 @@
         <v>24</v>
       </c>
       <c r="N60" s="11" t="s">
-        <v>1265</v>
+        <v>1252</v>
       </c>
       <c r="O60" s="11"/>
       <c r="P60" s="21" t="s">
@@ -8784,9 +8264,11 @@
       <c r="Q60" s="46">
         <v>44208</v>
       </c>
-      <c r="R60" s="46"/>
+      <c r="R60" s="46" t="s">
+        <v>1239</v>
+      </c>
       <c r="S60" s="21" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="61" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8829,12 +8311,22 @@
       <c r="M61" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N61" s="11"/>
+      <c r="N61" s="11" t="s">
+        <v>1253</v>
+      </c>
       <c r="O61" s="11"/>
-      <c r="P61" s="21"/>
-      <c r="Q61" s="46"/>
-      <c r="R61" s="46"/>
-      <c r="S61" s="21"/>
+      <c r="P61" s="21" t="s">
+        <v>1232</v>
+      </c>
+      <c r="Q61" s="46">
+        <v>44208</v>
+      </c>
+      <c r="R61" s="46" t="s">
+        <v>1239</v>
+      </c>
+      <c r="S61" s="21" t="s">
+        <v>1260</v>
+      </c>
     </row>
     <row r="62" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="26">
@@ -8876,12 +8368,22 @@
       <c r="M62" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N62" s="11"/>
+      <c r="N62" s="11" t="s">
+        <v>1254</v>
+      </c>
       <c r="O62" s="11"/>
-      <c r="P62" s="21"/>
-      <c r="Q62" s="46"/>
-      <c r="R62" s="46"/>
-      <c r="S62" s="21"/>
+      <c r="P62" s="21" t="s">
+        <v>1232</v>
+      </c>
+      <c r="Q62" s="46">
+        <v>44208</v>
+      </c>
+      <c r="R62" s="46" t="s">
+        <v>1239</v>
+      </c>
+      <c r="S62" s="21" t="s">
+        <v>1260</v>
+      </c>
     </row>
     <row r="63" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="28">
@@ -8924,22 +8426,22 @@
         <v>24</v>
       </c>
       <c r="N63" s="11" t="s">
-        <v>1212</v>
+        <v>1281</v>
       </c>
       <c r="O63" s="11" t="s">
         <v>1066</v>
       </c>
       <c r="P63" s="21" t="s">
-        <v>1256</v>
+        <v>1232</v>
       </c>
       <c r="Q63" s="46">
-        <v>44182</v>
+        <v>44208</v>
       </c>
       <c r="R63" s="46" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="S63" s="21" t="s">
-        <v>1255</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="64" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8984,10 +8486,16 @@
       </c>
       <c r="N64" s="11"/>
       <c r="O64" s="11"/>
-      <c r="P64" s="21"/>
-      <c r="Q64" s="46"/>
+      <c r="P64" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q64" s="46">
+        <v>44208</v>
+      </c>
       <c r="R64" s="46"/>
-      <c r="S64" s="21"/>
+      <c r="S64" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="65" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="29">
@@ -9030,22 +8538,22 @@
         <v>24</v>
       </c>
       <c r="N65" s="11" t="s">
-        <v>1212</v>
+        <v>1283</v>
       </c>
       <c r="O65" s="11" t="s">
         <v>1066</v>
       </c>
       <c r="P65" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q65" s="46">
+        <v>44208</v>
+      </c>
+      <c r="R65" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S65" s="21" t="s">
         <v>1256</v>
-      </c>
-      <c r="Q65" s="46">
-        <v>44182</v>
-      </c>
-      <c r="R65" s="46" t="s">
-        <v>1243</v>
-      </c>
-      <c r="S65" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="66" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9088,8 +8596,9 @@
       <c r="M66" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N66" s="11" t="s">
-        <v>1213</v>
+      <c r="N66" s="11" t="str">
+        <f>"opdracht_"&amp;B66&amp;".zip"</f>
+        <v>opdracht_LVBB1505.zip</v>
       </c>
       <c r="O66" s="11" t="s">
         <v>1066</v>
@@ -9098,13 +8607,13 @@
         <v>84</v>
       </c>
       <c r="Q66" s="46">
-        <v>44182</v>
+        <v>44208</v>
       </c>
       <c r="R66" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S66" s="21" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="67" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9147,23 +8656,24 @@
       <c r="M67" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N67" s="21" t="s">
-        <v>1213</v>
+      <c r="N67" s="21" t="str">
+        <f t="shared" ref="N67:N91" si="0">"opdracht_"&amp;B67&amp;".zip"</f>
+        <v>opdracht_LVBB1506.zip</v>
       </c>
       <c r="O67" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P67" s="21" t="s">
-        <v>84</v>
+        <v>1232</v>
       </c>
       <c r="Q67" s="46">
-        <v>44182</v>
+        <v>44208</v>
       </c>
       <c r="R67" s="46" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="S67" s="21" t="s">
-        <v>1257</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9206,23 +8716,17 @@
       <c r="M68" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N68" s="21" t="s">
-        <v>1213</v>
-      </c>
+      <c r="N68" s="21"/>
       <c r="O68" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P68" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="Q68" s="46">
-        <v>44182</v>
-      </c>
-      <c r="R68" s="46" t="s">
-        <v>1243</v>
-      </c>
+      <c r="Q68" s="46"/>
+      <c r="R68" s="46"/>
       <c r="S68" s="21" t="s">
-        <v>1257</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9265,12 +8769,16 @@
       <c r="M69" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N69" s="11"/>
+      <c r="N69" s="21"/>
       <c r="O69" s="11"/>
-      <c r="P69" s="21"/>
+      <c r="P69" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q69" s="46"/>
       <c r="R69" s="46"/>
-      <c r="S69" s="21"/>
+      <c r="S69" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="70" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="29">
@@ -9312,12 +8820,16 @@
       <c r="M70" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N70" s="11"/>
+      <c r="N70" s="21"/>
       <c r="O70" s="11"/>
-      <c r="P70" s="21"/>
+      <c r="P70" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q70" s="46"/>
       <c r="R70" s="46"/>
-      <c r="S70" s="21"/>
+      <c r="S70" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="71" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="29">
@@ -9359,8 +8871,9 @@
       <c r="M71" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N71" s="21" t="s">
-        <v>1213</v>
+      <c r="N71" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>opdracht_LVBB1510.zip</v>
       </c>
       <c r="O71" s="21" t="s">
         <v>1066</v>
@@ -9369,13 +8882,13 @@
         <v>84</v>
       </c>
       <c r="Q71" s="46">
-        <v>44182</v>
+        <v>44208</v>
       </c>
       <c r="R71" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S71" s="21" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="72" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9418,23 +8931,24 @@
       <c r="M72" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N72" s="21" t="s">
-        <v>1213</v>
+      <c r="N72" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>opdracht_LVBB1511.zip</v>
       </c>
       <c r="O72" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P72" s="21" t="s">
-        <v>84</v>
+        <v>1232</v>
       </c>
       <c r="Q72" s="46">
-        <v>44182</v>
+        <v>44208</v>
       </c>
       <c r="R72" s="46" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="S72" s="21" t="s">
-        <v>1257</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="73" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9477,18 +8991,22 @@
       <c r="M73" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N73" s="11"/>
+      <c r="N73" s="21"/>
       <c r="O73" s="11"/>
-      <c r="P73" s="21"/>
+      <c r="P73" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q73" s="46"/>
       <c r="R73" s="46"/>
-      <c r="S73" s="21"/>
+      <c r="S73" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="74" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
         <v>2</v>
       </c>
-      <c r="B74" s="40" t="s">
+      <c r="B74" s="15" t="s">
         <v>1075</v>
       </c>
       <c r="C74" s="21" t="s">
@@ -9524,12 +9042,16 @@
       <c r="M74" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="N74" s="11"/>
+      <c r="N74" s="21"/>
       <c r="O74" s="11"/>
-      <c r="P74" s="21"/>
+      <c r="P74" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q74" s="46"/>
       <c r="R74" s="46"/>
-      <c r="S74" s="21"/>
+      <c r="S74" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="75" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="29">
@@ -9571,23 +9093,24 @@
       <c r="M75" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N75" s="21" t="s">
-        <v>1212</v>
+      <c r="N75" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>opdracht_LVBB1514.zip</v>
       </c>
       <c r="O75" s="11" t="s">
         <v>1066</v>
       </c>
       <c r="P75" s="21" t="s">
-        <v>1256</v>
+        <v>1232</v>
       </c>
       <c r="Q75" s="46">
-        <v>44182</v>
+        <v>44208</v>
       </c>
       <c r="R75" s="46" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="S75" s="21" t="s">
-        <v>1255</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="76" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9630,12 +9153,16 @@
       <c r="M76" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N76" s="11"/>
+      <c r="N76" s="21"/>
       <c r="O76" s="11"/>
-      <c r="P76" s="21"/>
+      <c r="P76" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q76" s="46"/>
       <c r="R76" s="46"/>
-      <c r="S76" s="21"/>
+      <c r="S76" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="77" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="29">
@@ -9677,12 +9204,16 @@
       <c r="M77" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N77" s="11"/>
+      <c r="N77" s="21"/>
       <c r="O77" s="11"/>
-      <c r="P77" s="21"/>
+      <c r="P77" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q77" s="46"/>
       <c r="R77" s="46"/>
-      <c r="S77" s="21"/>
+      <c r="S77" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="78" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="29">
@@ -9724,12 +9255,16 @@
       <c r="M78" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N78" s="11"/>
+      <c r="N78" s="21"/>
       <c r="O78" s="11"/>
-      <c r="P78" s="21"/>
+      <c r="P78" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q78" s="46"/>
       <c r="R78" s="46"/>
-      <c r="S78" s="21"/>
+      <c r="S78" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="79" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="29">
@@ -9771,12 +9306,16 @@
       <c r="M79" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N79" s="11"/>
+      <c r="N79" s="21"/>
       <c r="O79" s="11"/>
-      <c r="P79" s="21"/>
+      <c r="P79" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q79" s="46"/>
       <c r="R79" s="46"/>
-      <c r="S79" s="21"/>
+      <c r="S79" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="80" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="29">
@@ -9818,12 +9357,16 @@
       <c r="M80" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N80" s="11"/>
+      <c r="N80" s="21"/>
       <c r="O80" s="11"/>
-      <c r="P80" s="21"/>
+      <c r="P80" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q80" s="46"/>
       <c r="R80" s="46"/>
-      <c r="S80" s="21"/>
+      <c r="S80" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="81" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="29">
@@ -9865,12 +9408,16 @@
       <c r="M81" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N81" s="11"/>
+      <c r="N81" s="21"/>
       <c r="O81" s="11"/>
-      <c r="P81" s="21"/>
+      <c r="P81" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q81" s="46"/>
       <c r="R81" s="46"/>
-      <c r="S81" s="21"/>
+      <c r="S81" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="82" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="29">
@@ -9912,12 +9459,16 @@
       <c r="M82" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N82" s="11"/>
+      <c r="N82" s="21"/>
       <c r="O82" s="11"/>
-      <c r="P82" s="21"/>
+      <c r="P82" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q82" s="46"/>
       <c r="R82" s="46"/>
-      <c r="S82" s="21"/>
+      <c r="S82" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="83" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="29">
@@ -9959,12 +9510,16 @@
       <c r="M83" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N83" s="11"/>
+      <c r="N83" s="21"/>
       <c r="O83" s="11"/>
-      <c r="P83" s="21"/>
+      <c r="P83" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q83" s="46"/>
       <c r="R83" s="46"/>
-      <c r="S83" s="21"/>
+      <c r="S83" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="84" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="29">
@@ -10006,14 +9561,22 @@
       <c r="M84" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N84" s="11"/>
+      <c r="N84" s="21"/>
       <c r="O84" s="11" t="s">
         <v>1066</v>
       </c>
-      <c r="P84" s="21"/>
-      <c r="Q84" s="46"/>
-      <c r="R84" s="46"/>
-      <c r="S84" s="21"/>
+      <c r="P84" s="21" t="s">
+        <v>1244</v>
+      </c>
+      <c r="Q84" s="46">
+        <v>44208</v>
+      </c>
+      <c r="R84" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S84" s="21" t="s">
+        <v>1285</v>
+      </c>
     </row>
     <row r="85" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="28">
@@ -10055,12 +9618,16 @@
       <c r="M85" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N85" s="11"/>
+      <c r="N85" s="21"/>
       <c r="O85" s="11"/>
-      <c r="P85" s="21"/>
+      <c r="P85" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q85" s="46"/>
       <c r="R85" s="46"/>
-      <c r="S85" s="21"/>
+      <c r="S85" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="86" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="28">
@@ -10102,8 +9669,9 @@
       <c r="M86" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N86" s="11" t="s">
-        <v>1211</v>
+      <c r="N86" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>opdracht_LVBB2003.zip</v>
       </c>
       <c r="O86" s="11" t="s">
         <v>1066</v>
@@ -10112,11 +9680,13 @@
         <v>1232</v>
       </c>
       <c r="Q86" s="46">
-        <v>44166</v>
-      </c>
-      <c r="R86" s="46"/>
+        <v>44208</v>
+      </c>
+      <c r="R86" s="46" t="s">
+        <v>1239</v>
+      </c>
       <c r="S86" s="21" t="s">
-        <v>1235</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="87" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10159,12 +9729,16 @@
       <c r="M87" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N87" s="11"/>
+      <c r="N87" s="21"/>
       <c r="O87" s="11"/>
-      <c r="P87" s="21"/>
+      <c r="P87" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="Q87" s="46"/>
       <c r="R87" s="46"/>
-      <c r="S87" s="21"/>
+      <c r="S87" s="21" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="88" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="26">
@@ -10206,23 +9780,24 @@
       <c r="M88" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N88" s="21" t="s">
-        <v>1212</v>
+      <c r="N88" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>opdracht_LVBB2006.zip</v>
       </c>
       <c r="O88" s="11" t="s">
         <v>1066</v>
       </c>
       <c r="P88" s="21" t="s">
-        <v>1256</v>
+        <v>1232</v>
       </c>
       <c r="Q88" s="46">
-        <v>44182</v>
+        <v>44208</v>
       </c>
       <c r="R88" s="46" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="S88" s="21" t="s">
-        <v>1255</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="89" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10265,23 +9840,24 @@
       <c r="M89" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N89" s="21" t="s">
-        <v>1212</v>
+      <c r="N89" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>opdracht_LVBB2007.zip</v>
       </c>
       <c r="O89" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P89" s="21" t="s">
-        <v>1256</v>
+        <v>1232</v>
       </c>
       <c r="Q89" s="46">
-        <v>44182</v>
+        <v>44208</v>
       </c>
       <c r="R89" s="46" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="S89" s="21" t="s">
-        <v>1255</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="90" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10324,23 +9900,24 @@
       <c r="M90" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N90" s="21" t="s">
-        <v>1212</v>
+      <c r="N90" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>opdracht_LVBB2008.zip</v>
       </c>
       <c r="O90" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P90" s="21" t="s">
-        <v>1256</v>
+        <v>1232</v>
       </c>
       <c r="Q90" s="46">
-        <v>44182</v>
+        <v>44208</v>
       </c>
       <c r="R90" s="46" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="S90" s="21" t="s">
-        <v>1255</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="91" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10383,23 +9960,24 @@
       <c r="M91" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N91" s="21" t="s">
-        <v>1212</v>
+      <c r="N91" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>opdracht_LVBB2009.zip</v>
       </c>
       <c r="O91" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P91" s="21" t="s">
-        <v>1256</v>
+        <v>1232</v>
       </c>
       <c r="Q91" s="46">
-        <v>44182</v>
+        <v>44208</v>
       </c>
       <c r="R91" s="46" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="S91" s="21" t="s">
-        <v>1255</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="92" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10442,23 +10020,19 @@
       <c r="M92" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N92" s="21" t="s">
-        <v>1212</v>
-      </c>
+      <c r="N92" s="21"/>
       <c r="O92" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P92" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="Q92" s="46">
-        <v>44182</v>
-      </c>
+        <v>1244</v>
+      </c>
+      <c r="Q92" s="46"/>
       <c r="R92" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S92" s="21" t="s">
-        <v>1255</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="93" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10501,23 +10075,19 @@
       <c r="M93" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N93" s="21" t="s">
-        <v>1212</v>
-      </c>
+      <c r="N93" s="21"/>
       <c r="O93" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P93" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="Q93" s="46">
-        <v>44182</v>
-      </c>
+        <v>1244</v>
+      </c>
+      <c r="Q93" s="46"/>
       <c r="R93" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S93" s="21" t="s">
-        <v>1255</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="94" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10560,23 +10130,19 @@
       <c r="M94" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N94" s="21" t="s">
-        <v>1212</v>
-      </c>
+      <c r="N94" s="21"/>
       <c r="O94" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P94" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="Q94" s="46">
-        <v>44182</v>
-      </c>
+        <v>1244</v>
+      </c>
+      <c r="Q94" s="46"/>
       <c r="R94" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S94" s="21" t="s">
-        <v>1255</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="95" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10619,23 +10185,19 @@
       <c r="M95" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N95" s="21" t="s">
-        <v>1212</v>
-      </c>
+      <c r="N95" s="21"/>
       <c r="O95" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P95" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="Q95" s="46">
-        <v>44182</v>
-      </c>
+        <v>1244</v>
+      </c>
+      <c r="Q95" s="46"/>
       <c r="R95" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S95" s="21" t="s">
-        <v>1255</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="96" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10678,23 +10240,19 @@
       <c r="M96" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N96" s="21" t="s">
-        <v>1212</v>
-      </c>
+      <c r="N96" s="21"/>
       <c r="O96" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P96" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="Q96" s="46">
-        <v>44182</v>
-      </c>
+        <v>1244</v>
+      </c>
+      <c r="Q96" s="46"/>
       <c r="R96" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S96" s="21" t="s">
-        <v>1255</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="97" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10737,23 +10295,19 @@
       <c r="M97" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N97" s="21" t="s">
-        <v>1212</v>
-      </c>
+      <c r="N97" s="21"/>
       <c r="O97" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P97" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="Q97" s="46">
-        <v>44182</v>
-      </c>
+        <v>1244</v>
+      </c>
+      <c r="Q97" s="46"/>
       <c r="R97" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S97" s="21" t="s">
-        <v>1255</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="98" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10796,23 +10350,19 @@
       <c r="M98" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N98" s="21" t="s">
-        <v>1212</v>
-      </c>
+      <c r="N98" s="21"/>
       <c r="O98" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P98" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="Q98" s="46">
-        <v>44182</v>
-      </c>
+        <v>1244</v>
+      </c>
+      <c r="Q98" s="46"/>
       <c r="R98" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S98" s="21" t="s">
-        <v>1255</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="99" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10855,23 +10405,19 @@
       <c r="M99" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N99" s="21" t="s">
-        <v>1212</v>
-      </c>
+      <c r="N99" s="21"/>
       <c r="O99" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P99" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="Q99" s="46">
-        <v>44182</v>
-      </c>
+        <v>1244</v>
+      </c>
+      <c r="Q99" s="46"/>
       <c r="R99" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S99" s="21" t="s">
-        <v>1255</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="100" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10914,23 +10460,19 @@
       <c r="M100" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N100" s="21" t="s">
-        <v>1212</v>
-      </c>
+      <c r="N100" s="21"/>
       <c r="O100" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P100" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="Q100" s="46">
-        <v>44182</v>
-      </c>
+        <v>1244</v>
+      </c>
+      <c r="Q100" s="46"/>
       <c r="R100" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S100" s="21" t="s">
-        <v>1255</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="101" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10973,23 +10515,19 @@
       <c r="M101" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N101" s="21" t="s">
-        <v>1212</v>
-      </c>
+      <c r="N101" s="21"/>
       <c r="O101" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P101" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="Q101" s="46">
-        <v>44182</v>
-      </c>
+        <v>1244</v>
+      </c>
+      <c r="Q101" s="46"/>
       <c r="R101" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S101" s="21" t="s">
-        <v>1255</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="102" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11032,23 +10570,19 @@
       <c r="M102" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N102" s="21" t="s">
-        <v>1212</v>
-      </c>
+      <c r="N102" s="21"/>
       <c r="O102" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P102" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="Q102" s="46">
-        <v>44182</v>
-      </c>
+        <v>1244</v>
+      </c>
+      <c r="Q102" s="46"/>
       <c r="R102" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S102" s="21" t="s">
-        <v>1255</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="103" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11091,23 +10625,19 @@
       <c r="M103" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N103" s="21" t="s">
-        <v>1212</v>
-      </c>
+      <c r="N103" s="21"/>
       <c r="O103" s="21" t="s">
         <v>1066</v>
       </c>
       <c r="P103" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="Q103" s="46">
-        <v>44182</v>
-      </c>
+        <v>1244</v>
+      </c>
+      <c r="Q103" s="46"/>
       <c r="R103" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S103" s="21" t="s">
-        <v>1255</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="104" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11493,7 +11023,7 @@
       </c>
       <c r="R111" s="46"/>
       <c r="S111" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="112" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11590,16 +11120,16 @@
         <v>1066</v>
       </c>
       <c r="P113" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q113" s="46">
         <v>44182</v>
       </c>
       <c r="R113" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S113" s="21" t="s">
         <v>1243</v>
-      </c>
-      <c r="S113" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="114" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11656,7 +11186,7 @@
       </c>
       <c r="R114" s="46"/>
       <c r="S114" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="115" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11713,7 +11243,7 @@
       </c>
       <c r="R115" s="46"/>
       <c r="S115" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="116" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11770,7 +11300,7 @@
       </c>
       <c r="R116" s="46"/>
       <c r="S116" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="117" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11921,7 +11451,7 @@
       </c>
       <c r="R119" s="46"/>
       <c r="S119" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="120" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11978,7 +11508,7 @@
       </c>
       <c r="R120" s="46"/>
       <c r="S120" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="121" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12035,7 +11565,7 @@
       </c>
       <c r="R121" s="46"/>
       <c r="S121" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="122" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12092,7 +11622,7 @@
       </c>
       <c r="R122" s="46"/>
       <c r="S122" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="123" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12149,7 +11679,7 @@
       </c>
       <c r="R123" s="46"/>
       <c r="S123" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="124" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12253,7 +11783,7 @@
       </c>
       <c r="R125" s="46"/>
       <c r="S125" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="126" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12303,16 +11833,16 @@
         <v>1066</v>
       </c>
       <c r="P126" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q126" s="46">
         <v>44182</v>
       </c>
       <c r="R126" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S126" s="21" t="s">
         <v>1243</v>
-      </c>
-      <c r="S126" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="127" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12362,16 +11892,16 @@
         <v>1066</v>
       </c>
       <c r="P127" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q127" s="46">
         <v>44182</v>
       </c>
       <c r="R127" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S127" s="21" t="s">
         <v>1243</v>
-      </c>
-      <c r="S127" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="128" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12421,16 +11951,16 @@
         <v>1066</v>
       </c>
       <c r="P128" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q128" s="46">
         <v>44182</v>
       </c>
       <c r="R128" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S128" s="21" t="s">
         <v>1243</v>
-      </c>
-      <c r="S128" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="129" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12480,16 +12010,16 @@
         <v>1066</v>
       </c>
       <c r="P129" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q129" s="46">
         <v>44182</v>
       </c>
       <c r="R129" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S129" s="21" t="s">
         <v>1243</v>
-      </c>
-      <c r="S129" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="130" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12539,16 +12069,16 @@
         <v>1066</v>
       </c>
       <c r="P130" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q130" s="46">
         <v>44182</v>
       </c>
       <c r="R130" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S130" s="21" t="s">
         <v>1243</v>
-      </c>
-      <c r="S130" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="131" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12741,16 +12271,16 @@
         <v>1066</v>
       </c>
       <c r="P134" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q134" s="46">
         <v>44182</v>
       </c>
       <c r="R134" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S134" s="21" t="s">
         <v>1243</v>
-      </c>
-      <c r="S134" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="135" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12800,16 +12330,16 @@
         <v>1066</v>
       </c>
       <c r="P135" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q135" s="46">
         <v>44182</v>
       </c>
       <c r="R135" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S135" s="21" t="s">
         <v>1243</v>
-      </c>
-      <c r="S135" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="136" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13102,10 +12632,10 @@
         <v>44182</v>
       </c>
       <c r="R141" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S141" s="21" t="s">
-        <v>1257</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="142" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13249,16 +12779,16 @@
         <v>1066</v>
       </c>
       <c r="P144" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q144" s="46">
         <v>44182</v>
       </c>
       <c r="R144" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S144" s="21" t="s">
         <v>1243</v>
-      </c>
-      <c r="S144" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="145" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13355,16 +12885,16 @@
         <v>1066</v>
       </c>
       <c r="P146" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q146" s="46">
         <v>44182</v>
       </c>
       <c r="R146" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S146" s="21" t="s">
         <v>1243</v>
-      </c>
-      <c r="S146" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="147" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13414,16 +12944,16 @@
         <v>1066</v>
       </c>
       <c r="P147" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q147" s="46">
         <v>44182</v>
       </c>
       <c r="R147" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S147" s="21" t="s">
         <v>1243</v>
-      </c>
-      <c r="S147" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="148" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13473,16 +13003,16 @@
         <v>1066</v>
       </c>
       <c r="P148" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q148" s="46">
         <v>44166</v>
       </c>
       <c r="R148" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S148" s="21" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="149" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13532,16 +13062,16 @@
         <v>1066</v>
       </c>
       <c r="P149" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q149" s="46">
         <v>44166</v>
       </c>
       <c r="R149" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S149" s="21" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="150" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13591,16 +13121,16 @@
         <v>1066</v>
       </c>
       <c r="P150" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q150" s="46">
         <v>44166</v>
       </c>
       <c r="R150" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S150" s="21" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="151" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13697,16 +13227,16 @@
         <v>1066</v>
       </c>
       <c r="P152" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q152" s="46">
         <v>44166</v>
       </c>
       <c r="R152" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S152" s="21" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="153" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13844,7 +13374,7 @@
         <v>24</v>
       </c>
       <c r="N155" s="21" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="O155" s="25" t="s">
         <v>1066</v>
@@ -13907,10 +13437,10 @@
         <v>44182</v>
       </c>
       <c r="R156" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S156" s="21" t="s">
-        <v>1257</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="157" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13966,10 +13496,10 @@
         <v>44182</v>
       </c>
       <c r="R157" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S157" s="21" t="s">
-        <v>1257</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="158" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14065,16 +13595,16 @@
         <v>1066</v>
       </c>
       <c r="P159" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q159" s="46">
         <v>44166</v>
       </c>
       <c r="R159" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S159" s="21" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="160" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14218,16 +13748,16 @@
         <v>1066</v>
       </c>
       <c r="P162" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q162" s="46">
         <v>44182</v>
       </c>
       <c r="R162" s="46" t="s">
+        <v>1241</v>
+      </c>
+      <c r="S162" s="21" t="s">
         <v>1243</v>
-      </c>
-      <c r="S162" s="21" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="163" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14418,16 +13948,16 @@
         <v>1066</v>
       </c>
       <c r="P166" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q166" s="46">
         <v>44166</v>
       </c>
       <c r="R166" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S166" s="21" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="167" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14477,16 +14007,16 @@
         <v>1066</v>
       </c>
       <c r="P167" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q167" s="46">
         <v>44166</v>
       </c>
       <c r="R167" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S167" s="21" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="168" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14542,10 +14072,10 @@
         <v>44182</v>
       </c>
       <c r="R168" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S168" s="21" t="s">
-        <v>1257</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="169" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14642,16 +14172,16 @@
         <v>1066</v>
       </c>
       <c r="P170" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q170" s="46">
         <v>44182</v>
       </c>
       <c r="R170" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S170" s="21" t="s">
-        <v>1258</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="171" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14701,16 +14231,16 @@
         <v>1066</v>
       </c>
       <c r="P171" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q171" s="46">
         <v>44182</v>
       </c>
       <c r="R171" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S171" s="21" t="s">
-        <v>1258</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="172" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14760,16 +14290,16 @@
         <v>1066</v>
       </c>
       <c r="P172" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q172" s="46">
         <v>44182</v>
       </c>
       <c r="R172" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S172" s="21" t="s">
-        <v>1258</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="173" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17035,7 +16565,7 @@
       </c>
       <c r="R220" s="46"/>
       <c r="S220" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="221" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17132,14 +16662,14 @@
         <v>1066</v>
       </c>
       <c r="P222" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q222" s="46">
         <v>44166</v>
       </c>
       <c r="R222" s="46"/>
       <c r="S222" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="223" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17189,14 +16719,14 @@
         <v>1066</v>
       </c>
       <c r="P223" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q223" s="46">
         <v>44166</v>
       </c>
       <c r="R223" s="46"/>
       <c r="S223" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="224" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17246,14 +16776,14 @@
         <v>1066</v>
       </c>
       <c r="P224" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q224" s="46">
         <v>44166</v>
       </c>
       <c r="R224" s="46"/>
       <c r="S224" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="225" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17303,14 +16833,14 @@
         <v>1066</v>
       </c>
       <c r="P225" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q225" s="46">
         <v>44166</v>
       </c>
       <c r="R225" s="46"/>
       <c r="S225" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="226" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17360,14 +16890,14 @@
         <v>1066</v>
       </c>
       <c r="P226" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q226" s="46">
         <v>44166</v>
       </c>
       <c r="R226" s="46"/>
       <c r="S226" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="227" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17417,14 +16947,14 @@
         <v>1066</v>
       </c>
       <c r="P227" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q227" s="46">
         <v>44166</v>
       </c>
       <c r="R227" s="46"/>
       <c r="S227" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="228" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17474,14 +17004,14 @@
         <v>1066</v>
       </c>
       <c r="P228" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q228" s="46">
         <v>44166</v>
       </c>
       <c r="R228" s="46"/>
       <c r="S228" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="229" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17531,14 +17061,14 @@
         <v>1066</v>
       </c>
       <c r="P229" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q229" s="46">
         <v>44166</v>
       </c>
       <c r="R229" s="46"/>
       <c r="S229" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="230" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17588,14 +17118,14 @@
         <v>1066</v>
       </c>
       <c r="P230" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q230" s="46">
         <v>44166</v>
       </c>
       <c r="R230" s="46"/>
       <c r="S230" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="231" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17645,14 +17175,14 @@
         <v>1066</v>
       </c>
       <c r="P231" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q231" s="46">
         <v>44166</v>
       </c>
       <c r="R231" s="46"/>
       <c r="S231" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="232" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17702,14 +17232,14 @@
         <v>1066</v>
       </c>
       <c r="P232" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q232" s="46">
         <v>44166</v>
       </c>
       <c r="R232" s="46"/>
       <c r="S232" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="233" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17759,14 +17289,14 @@
         <v>1066</v>
       </c>
       <c r="P233" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q233" s="46">
         <v>44166</v>
       </c>
       <c r="R233" s="46"/>
       <c r="S233" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="234" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17816,14 +17346,14 @@
         <v>1066</v>
       </c>
       <c r="P234" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q234" s="46">
         <v>44166</v>
       </c>
       <c r="R234" s="46"/>
       <c r="S234" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="235" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17873,14 +17403,14 @@
         <v>1066</v>
       </c>
       <c r="P235" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q235" s="46">
         <v>44166</v>
       </c>
       <c r="R235" s="46"/>
       <c r="S235" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="236" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17930,14 +17460,14 @@
         <v>1066</v>
       </c>
       <c r="P236" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q236" s="46">
         <v>44166</v>
       </c>
       <c r="R236" s="46"/>
       <c r="S236" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="237" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17987,14 +17517,14 @@
         <v>1066</v>
       </c>
       <c r="P237" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q237" s="46">
         <v>44166</v>
       </c>
       <c r="R237" s="46"/>
       <c r="S237" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="238" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18044,14 +17574,14 @@
         <v>1066</v>
       </c>
       <c r="P238" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q238" s="46">
         <v>44166</v>
       </c>
       <c r="R238" s="46"/>
       <c r="S238" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="239" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18101,14 +17631,14 @@
         <v>1066</v>
       </c>
       <c r="P239" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q239" s="46">
         <v>44166</v>
       </c>
       <c r="R239" s="46"/>
       <c r="S239" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="240" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18158,14 +17688,14 @@
         <v>1066</v>
       </c>
       <c r="P240" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q240" s="46">
         <v>44166</v>
       </c>
       <c r="R240" s="46"/>
       <c r="S240" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="241" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18215,14 +17745,14 @@
         <v>1066</v>
       </c>
       <c r="P241" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q241" s="46">
         <v>44166</v>
       </c>
       <c r="R241" s="46"/>
       <c r="S241" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="242" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18272,14 +17802,14 @@
         <v>1066</v>
       </c>
       <c r="P242" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q242" s="46">
         <v>44166</v>
       </c>
       <c r="R242" s="46"/>
       <c r="S242" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="243" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18329,14 +17859,14 @@
         <v>1066</v>
       </c>
       <c r="P243" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q243" s="46">
         <v>44166</v>
       </c>
       <c r="R243" s="46"/>
       <c r="S243" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="244" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18386,14 +17916,14 @@
         <v>1066</v>
       </c>
       <c r="P244" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q244" s="46">
         <v>44166</v>
       </c>
       <c r="R244" s="46"/>
       <c r="S244" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="245" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18443,14 +17973,14 @@
         <v>1066</v>
       </c>
       <c r="P245" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q245" s="46">
         <v>44166</v>
       </c>
       <c r="R245" s="46"/>
       <c r="S245" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="246" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18500,14 +18030,14 @@
         <v>1066</v>
       </c>
       <c r="P246" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q246" s="46">
         <v>44166</v>
       </c>
       <c r="R246" s="46"/>
       <c r="S246" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="247" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18557,14 +18087,14 @@
         <v>1066</v>
       </c>
       <c r="P247" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q247" s="46">
         <v>44166</v>
       </c>
       <c r="R247" s="46"/>
       <c r="S247" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="248" spans="1:19" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18614,14 +18144,14 @@
         <v>1066</v>
       </c>
       <c r="P248" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q248" s="46">
         <v>44166</v>
       </c>
       <c r="R248" s="46"/>
       <c r="S248" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="249" spans="1:19" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18671,14 +18201,14 @@
         <v>1066</v>
       </c>
       <c r="P249" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q249" s="46">
         <v>44166</v>
       </c>
       <c r="R249" s="46"/>
       <c r="S249" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="250" spans="1:19" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18728,14 +18258,14 @@
         <v>1066</v>
       </c>
       <c r="P250" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q250" s="46">
         <v>44166</v>
       </c>
       <c r="R250" s="46"/>
       <c r="S250" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="251" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18785,14 +18315,14 @@
         <v>1066</v>
       </c>
       <c r="P251" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q251" s="46">
         <v>44166</v>
       </c>
       <c r="R251" s="46"/>
       <c r="S251" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="252" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18842,14 +18372,14 @@
         <v>1066</v>
       </c>
       <c r="P252" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q252" s="46">
         <v>44166</v>
       </c>
       <c r="R252" s="46"/>
       <c r="S252" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="253" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18899,14 +18429,14 @@
         <v>1066</v>
       </c>
       <c r="P253" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q253" s="46">
         <v>44166</v>
       </c>
       <c r="R253" s="46"/>
       <c r="S253" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="254" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18956,14 +18486,14 @@
         <v>1066</v>
       </c>
       <c r="P254" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q254" s="46">
         <v>44166</v>
       </c>
       <c r="R254" s="46"/>
       <c r="S254" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="255" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19013,14 +18543,14 @@
         <v>1066</v>
       </c>
       <c r="P255" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q255" s="46">
         <v>44166</v>
       </c>
       <c r="R255" s="46"/>
       <c r="S255" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="256" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19070,14 +18600,14 @@
         <v>1066</v>
       </c>
       <c r="P256" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q256" s="46">
         <v>44166</v>
       </c>
       <c r="R256" s="46"/>
       <c r="S256" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="257" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19127,14 +18657,14 @@
         <v>1066</v>
       </c>
       <c r="P257" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q257" s="46">
         <v>44166</v>
       </c>
       <c r="R257" s="46"/>
       <c r="S257" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="258" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19184,14 +18714,14 @@
         <v>1066</v>
       </c>
       <c r="P258" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q258" s="46">
         <v>44166</v>
       </c>
       <c r="R258" s="46"/>
       <c r="S258" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="259" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19241,14 +18771,14 @@
         <v>1066</v>
       </c>
       <c r="P259" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q259" s="46">
         <v>44166</v>
       </c>
       <c r="R259" s="46"/>
       <c r="S259" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="260" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19298,14 +18828,14 @@
         <v>1066</v>
       </c>
       <c r="P260" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q260" s="46">
         <v>44166</v>
       </c>
       <c r="R260" s="46"/>
       <c r="S260" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="261" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19355,14 +18885,14 @@
         <v>1066</v>
       </c>
       <c r="P261" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q261" s="46">
         <v>44166</v>
       </c>
       <c r="R261" s="46"/>
       <c r="S261" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="262" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19412,14 +18942,14 @@
         <v>1066</v>
       </c>
       <c r="P262" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q262" s="46">
         <v>44166</v>
       </c>
       <c r="R262" s="46"/>
       <c r="S262" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="263" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19469,14 +18999,14 @@
         <v>1066</v>
       </c>
       <c r="P263" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q263" s="46">
         <v>44166</v>
       </c>
       <c r="R263" s="46"/>
       <c r="S263" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="264" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19526,14 +19056,14 @@
         <v>1066</v>
       </c>
       <c r="P264" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q264" s="46">
         <v>44166</v>
       </c>
       <c r="R264" s="46"/>
       <c r="S264" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="265" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19583,14 +19113,14 @@
         <v>1066</v>
       </c>
       <c r="P265" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q265" s="46">
         <v>44166</v>
       </c>
       <c r="R265" s="46"/>
       <c r="S265" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="266" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19640,14 +19170,14 @@
         <v>1066</v>
       </c>
       <c r="P266" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q266" s="46">
         <v>44166</v>
       </c>
       <c r="R266" s="46"/>
       <c r="S266" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="267" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19697,14 +19227,14 @@
         <v>1066</v>
       </c>
       <c r="P267" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q267" s="46">
         <v>44166</v>
       </c>
       <c r="R267" s="46"/>
       <c r="S267" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="268" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19807,10 +19337,10 @@
         <v>44182</v>
       </c>
       <c r="R269" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S269" s="21" t="s">
-        <v>1257</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="270" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19866,10 +19396,10 @@
         <v>44182</v>
       </c>
       <c r="R270" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S270" s="21" t="s">
-        <v>1257</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="271" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19925,10 +19455,10 @@
         <v>44182</v>
       </c>
       <c r="R271" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S271" s="21" t="s">
-        <v>1257</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="272" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19978,14 +19508,14 @@
         <v>1066</v>
       </c>
       <c r="P272" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q272" s="46">
         <v>44166</v>
       </c>
       <c r="R272" s="46"/>
       <c r="S272" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="273" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20035,14 +19565,14 @@
         <v>1066</v>
       </c>
       <c r="P273" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q273" s="46">
         <v>44166</v>
       </c>
       <c r="R273" s="46"/>
       <c r="S273" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="274" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20186,14 +19716,14 @@
         <v>1066</v>
       </c>
       <c r="P276" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q276" s="46">
         <v>44166</v>
       </c>
       <c r="R276" s="46"/>
       <c r="S276" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="277" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20243,14 +19773,14 @@
         <v>1066</v>
       </c>
       <c r="P277" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q277" s="46">
         <v>44166</v>
       </c>
       <c r="R277" s="46"/>
       <c r="S277" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="278" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20300,14 +19830,14 @@
         <v>1066</v>
       </c>
       <c r="P278" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q278" s="46">
         <v>44166</v>
       </c>
       <c r="R278" s="46"/>
       <c r="S278" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="279" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20357,14 +19887,14 @@
         <v>1066</v>
       </c>
       <c r="P279" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q279" s="46">
         <v>44166</v>
       </c>
       <c r="R279" s="46"/>
       <c r="S279" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="280" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20602,14 +20132,14 @@
         <v>1066</v>
       </c>
       <c r="P284" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q284" s="46">
         <v>44166</v>
       </c>
       <c r="R284" s="46"/>
       <c r="S284" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="285" spans="1:19" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20800,14 +20330,14 @@
         <v>1066</v>
       </c>
       <c r="P288" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q288" s="46">
         <v>44166</v>
       </c>
       <c r="R288" s="46"/>
       <c r="S288" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="289" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20857,14 +20387,14 @@
         <v>1066</v>
       </c>
       <c r="P289" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q289" s="46">
         <v>44166</v>
       </c>
       <c r="R289" s="46"/>
       <c r="S289" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="290" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20914,14 +20444,14 @@
         <v>1066</v>
       </c>
       <c r="P290" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q290" s="46">
         <v>44166</v>
       </c>
       <c r="R290" s="46"/>
       <c r="S290" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="291" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20971,14 +20501,14 @@
         <v>1066</v>
       </c>
       <c r="P291" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q291" s="46">
         <v>44166</v>
       </c>
       <c r="R291" s="46"/>
       <c r="S291" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="292" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21028,14 +20558,14 @@
         <v>1066</v>
       </c>
       <c r="P292" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q292" s="46">
         <v>44166</v>
       </c>
       <c r="R292" s="46"/>
       <c r="S292" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="293" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21085,14 +20615,14 @@
         <v>1066</v>
       </c>
       <c r="P293" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q293" s="46">
         <v>44166</v>
       </c>
       <c r="R293" s="46"/>
       <c r="S293" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="294" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21142,14 +20672,14 @@
         <v>1066</v>
       </c>
       <c r="P294" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q294" s="46">
         <v>44166</v>
       </c>
       <c r="R294" s="46"/>
       <c r="S294" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="295" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21205,10 +20735,10 @@
         <v>44182</v>
       </c>
       <c r="R295" s="46" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="S295" s="21" t="s">
-        <v>1257</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="296" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21258,14 +20788,14 @@
         <v>1066</v>
       </c>
       <c r="P296" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q296" s="46">
         <v>44166</v>
       </c>
       <c r="R296" s="46"/>
       <c r="S296" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="297" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21561,7 +21091,7 @@
       </c>
       <c r="R302" s="46"/>
       <c r="S302" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="303" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21618,7 +21148,7 @@
       </c>
       <c r="R303" s="46"/>
       <c r="S303" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="304" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21668,14 +21198,14 @@
         <v>1066</v>
       </c>
       <c r="P304" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q304" s="46">
         <v>44182</v>
       </c>
       <c r="R304" s="46"/>
       <c r="S304" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="305" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21725,14 +21255,14 @@
         <v>1066</v>
       </c>
       <c r="P305" s="21" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
       <c r="Q305" s="46">
         <v>44182</v>
       </c>
       <c r="R305" s="46"/>
       <c r="S305" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="306" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -22259,7 +21789,7 @@
       </c>
       <c r="R316" s="46"/>
       <c r="S316" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="317" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -22316,7 +21846,7 @@
       </c>
       <c r="R317" s="46"/>
       <c r="S317" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="318" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -22373,7 +21903,7 @@
       </c>
       <c r="R318" s="46"/>
       <c r="S318" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="319" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -22430,7 +21960,7 @@
       </c>
       <c r="R319" s="46"/>
       <c r="S319" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="320" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -22487,7 +22017,7 @@
       </c>
       <c r="R320" s="46"/>
       <c r="S320" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="321" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -22638,7 +22168,7 @@
       </c>
       <c r="R323" s="46"/>
       <c r="S323" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="324" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -22793,7 +22323,7 @@
       </c>
       <c r="R326" s="46"/>
       <c r="S326" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="327" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -22850,7 +22380,7 @@
       </c>
       <c r="R327" s="46"/>
       <c r="S327" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="328" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -22958,7 +22488,7 @@
       </c>
       <c r="R329" s="46"/>
       <c r="S329" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="330" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23015,7 +22545,7 @@
       </c>
       <c r="R330" s="46"/>
       <c r="S330" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="331" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23123,7 +22653,7 @@
       </c>
       <c r="R332" s="46"/>
       <c r="S332" s="21" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="333" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23180,7 +22710,7 @@
       </c>
       <c r="R333" s="46"/>
       <c r="S333" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="334" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23237,7 +22767,7 @@
       </c>
       <c r="R334" s="46"/>
       <c r="S334" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="335" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23294,7 +22824,7 @@
       </c>
       <c r="R335" s="46"/>
       <c r="S335" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="336" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23351,7 +22881,7 @@
       </c>
       <c r="R336" s="46"/>
       <c r="S336" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="337" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -31624,7 +31154,7 @@
       </c>
       <c r="R513" s="46"/>
       <c r="S513" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="514" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -31681,7 +31211,7 @@
       </c>
       <c r="R514" s="46"/>
       <c r="S514" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="515" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -31738,7 +31268,7 @@
       </c>
       <c r="R515" s="46"/>
       <c r="S515" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="516" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -31795,7 +31325,7 @@
       </c>
       <c r="R516" s="46"/>
       <c r="S516" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="517" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -31852,7 +31382,7 @@
       </c>
       <c r="R517" s="46"/>
       <c r="S517" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="518" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -31909,7 +31439,7 @@
       </c>
       <c r="R518" s="46"/>
       <c r="S518" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="519" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -31966,7 +31496,7 @@
       </c>
       <c r="R519" s="46"/>
       <c r="S519" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="520" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32023,7 +31553,7 @@
       </c>
       <c r="R520" s="46"/>
       <c r="S520" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="521" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32182,7 +31712,7 @@
       </c>
       <c r="R523" s="46"/>
       <c r="S523" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="524" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32239,7 +31769,7 @@
       </c>
       <c r="R524" s="46"/>
       <c r="S524" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="525" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32296,7 +31826,7 @@
       </c>
       <c r="R525" s="46"/>
       <c r="S525" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="526" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32353,7 +31883,7 @@
       </c>
       <c r="R526" s="46"/>
       <c r="S526" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="527" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32410,7 +31940,7 @@
       </c>
       <c r="R527" s="46"/>
       <c r="S527" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="528" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32467,7 +31997,7 @@
       </c>
       <c r="R528" s="46"/>
       <c r="S528" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="529" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32524,7 +32054,7 @@
       </c>
       <c r="R529" s="46"/>
       <c r="S529" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="530" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32581,7 +32111,7 @@
       </c>
       <c r="R530" s="46"/>
       <c r="S530" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="531" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32685,7 +32215,7 @@
       </c>
       <c r="R532" s="46"/>
       <c r="S532" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="533" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32742,7 +32272,7 @@
       </c>
       <c r="R533" s="46"/>
       <c r="S533" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="534" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32799,7 +32329,7 @@
       </c>
       <c r="R534" s="46"/>
       <c r="S534" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="535" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32856,7 +32386,7 @@
       </c>
       <c r="R535" s="46"/>
       <c r="S535" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="536" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32913,7 +32443,7 @@
       </c>
       <c r="R536" s="46"/>
       <c r="S536" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="537" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32970,7 +32500,7 @@
       </c>
       <c r="R537" s="46"/>
       <c r="S537" s="21" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="538" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -35247,7 +34777,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P54">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"nvt"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35578,12 +35108,12 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1 C1 A2:C37 A39:C1048576">
-    <cfRule type="containsText" dxfId="68" priority="31" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="6" priority="31" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:C38">
-    <cfRule type="containsText" dxfId="67" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A38)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>